<commit_message>
JPY work in progress
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/JPY_SynthQuotesFeed.xlsx
+++ b/QuantLibXL/Data2/XLS/JPY_SynthQuotesFeed.xlsx
@@ -1522,6 +1522,19 @@
     <xf numFmtId="165" fontId="9" fillId="0" borderId="24" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="26" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="46" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="19" xfId="11" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="11" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="20" xfId="11" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="15" xfId="11" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="175" fontId="18" fillId="9" borderId="13" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="18" fillId="9" borderId="13" xfId="11" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="21" xfId="11" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="22" xfId="11" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="23" xfId="11" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="16" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1552,19 +1565,6 @@
     <xf numFmtId="0" fontId="14" fillId="7" borderId="18" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="19" xfId="11" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="11" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="20" xfId="11" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="15" xfId="11" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="18" fillId="9" borderId="13" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="18" fillId="9" borderId="13" xfId="11" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="21" xfId="11" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="22" xfId="11" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="23" xfId="11" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="37">
     <cellStyle name="Euro" xfId="1"/>
@@ -1631,28 +1631,23 @@
       <sheetName val="Libor"/>
       <sheetName val="Tibor"/>
       <sheetName val="LiborSwapIsdaFixAm"/>
+      <sheetName val="LiborSwapIsdaFixPm"/>
       <sheetName val="LiborSwapForBasisCalc"/>
-      <sheetName val="LiborSwapIsdaFixPm"/>
+      <sheetName val="OIS"/>
       <sheetName val="BasisSwap1MxM"/>
       <sheetName val="BasisSwap3M6M"/>
-      <sheetName val="BasisSwapxM12M"/>
       <sheetName val="Deposits"/>
       <sheetName val="FRA"/>
-      <sheetName val="Futures1M"/>
+      <sheetName val="Futures3M_TIBOR"/>
       <sheetName val="Futures3M"/>
-      <sheetName val="ImmFra6M "/>
       <sheetName val="FuturesHWConvAdj"/>
-      <sheetName val="OIS"/>
       <sheetName val="Swaps1M"/>
-      <sheetName val="SwapsIMMDated"/>
+      <sheetName val="Swap3M_TIBOR"/>
       <sheetName val="Swap3M"/>
       <sheetName val="Swap6M"/>
       <sheetName val="ON"/>
       <sheetName val="1M (2)"/>
       <sheetName val="3M (2)"/>
-      <sheetName val="SFIX3"/>
-      <sheetName val="IB365"/>
-      <sheetName val="IBOR"/>
     </sheetNames>
     <definedNames>
       <definedName name="LastFixingsTrigger" refersTo="='General Settings'!$D$8"/>
@@ -1662,7 +1657,7 @@
       <sheetData sheetId="0">
         <row r="7">
           <cell r="D7">
-            <v>2</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="8">
@@ -1676,16 +1671,28 @@
       <sheetData sheetId="3">
         <row r="7">
           <cell r="D7" t="str">
-            <v>3M</v>
+            <v>6M</v>
           </cell>
         </row>
         <row r="8">
           <cell r="D8" t="str">
-            <v>3M</v>
+            <v>6M</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="4">
+        <row r="7">
+          <cell r="D7" t="str">
+            <v>6M</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="D8" t="str">
+            <v>6M</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="5">
         <row r="7">
           <cell r="D7" t="str">
             <v>Fwd Curve</v>
@@ -1697,27 +1704,15 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="5">
+      <sheetData sheetId="6">
         <row r="7">
           <cell r="D7" t="str">
-            <v>3M</v>
+            <v>3W</v>
           </cell>
         </row>
         <row r="8">
           <cell r="D8" t="str">
-            <v>3M</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="6">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>6L</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="D8" t="str">
-            <v>6L</v>
+            <v>1M</v>
           </cell>
         </row>
       </sheetData>
@@ -1736,12 +1731,12 @@
       <sheetData sheetId="8">
         <row r="7">
           <cell r="D7" t="str">
-            <v>12L</v>
+            <v>6L</v>
           </cell>
         </row>
         <row r="8">
           <cell r="D8" t="str">
-            <v>12L</v>
+            <v>6L</v>
           </cell>
         </row>
       </sheetData>
@@ -1793,32 +1788,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="13">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>V4</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="D8" t="str">
-            <v>X4</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>3W</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="D8" t="str">
-            <v>1M</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="16">
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14">
         <row r="7">
           <cell r="D7" t="str">
             <v>X1S</v>
@@ -1830,19 +1801,19 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="17">
+      <sheetData sheetId="15">
         <row r="7">
-          <cell r="D7">
-            <v>12</v>
+          <cell r="D7" t="str">
+            <v>3T</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="D8">
-            <v>12</v>
+          <cell r="D8" t="str">
+            <v>3T</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="18">
+      <sheetData sheetId="16">
         <row r="7">
           <cell r="D7" t="str">
             <v>3L</v>
@@ -1854,6 +1825,19 @@
           </cell>
         </row>
       </sheetData>
+      <sheetData sheetId="17">
+        <row r="7">
+          <cell r="D7" t="str">
+            <v>6L</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="D8" t="str">
+            <v>6L</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="18"/>
       <sheetData sheetId="19">
         <row r="7">
           <cell r="D7" t="str">
@@ -1866,8 +1850,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21">
+      <sheetData sheetId="20">
         <row r="7">
           <cell r="D7" t="str">
             <v>6L</v>
@@ -1876,54 +1859,6 @@
         <row r="8">
           <cell r="D8" t="str">
             <v>6L</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="22">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>6L</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="D8" t="str">
-            <v>6L</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="23">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>JPY-4Y=</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="D8" t="str">
-            <v>JPY-5Y=</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="24">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>JPY-SWD=</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="D8" t="str">
-            <v>JPY-2WD=</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="25">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>JPY-SWD=</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="D8" t="str">
-            <v>JPY-2WD=</v>
           </cell>
         </row>
       </sheetData>
@@ -2247,18 +2182,18 @@
       </c>
     </row>
     <row r="2" spans="1:35" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="241" t="s">
+      <c r="B2" s="250" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="242"/>
-      <c r="D2" s="242"/>
-      <c r="E2" s="243"/>
-      <c r="G2" s="244" t="s">
+      <c r="C2" s="251"/>
+      <c r="D2" s="251"/>
+      <c r="E2" s="252"/>
+      <c r="G2" s="253" t="s">
         <v>59</v>
       </c>
-      <c r="H2" s="245"/>
-      <c r="I2" s="245"/>
-      <c r="J2" s="246"/>
+      <c r="H2" s="254"/>
+      <c r="I2" s="254"/>
+      <c r="J2" s="255"/>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B3" s="133"/>
@@ -2486,22 +2421,22 @@
     </row>
     <row r="14" spans="1:35" ht="12" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:35" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="247" t="s">
+      <c r="B15" s="256" t="s">
         <v>87</v>
       </c>
-      <c r="C15" s="242" t="s">
+      <c r="C15" s="251" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="242"/>
-      <c r="E15" s="243"/>
-      <c r="G15" s="247" t="s">
+      <c r="D15" s="251"/>
+      <c r="E15" s="252"/>
+      <c r="G15" s="256" t="s">
         <v>86</v>
       </c>
-      <c r="H15" s="242" t="s">
+      <c r="H15" s="251" t="s">
         <v>86</v>
       </c>
-      <c r="I15" s="242"/>
-      <c r="J15" s="243"/>
+      <c r="I15" s="251"/>
+      <c r="J15" s="252"/>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B16" s="221"/>
@@ -2520,7 +2455,7 @@
       </c>
       <c r="D17" s="55">
         <f>_xll.qlCalendarAdvance(Calendar,EvaluationDate,"2D","f")</f>
-        <v>41800</v>
+        <v>41802</v>
       </c>
       <c r="E17" s="223"/>
       <c r="G17" s="221"/>
@@ -2528,7 +2463,7 @@
         <v>53</v>
       </c>
       <c r="I17" s="55">
-        <v>41796.72315972222</v>
+        <v>41800.738935185182</v>
       </c>
       <c r="J17" s="223"/>
     </row>
@@ -2539,7 +2474,7 @@
       </c>
       <c r="D18" s="55" t="str">
         <f>_xll.qlDiscountingSwapEngine(,OisCurve,,,,,EvaluationDate)</f>
-        <v>obj_00335#0001</v>
+        <v>obj_00378#0000</v>
       </c>
       <c r="E18" s="223"/>
       <c r="G18" s="221"/>
@@ -2548,7 +2483,7 @@
       </c>
       <c r="I18" s="55">
         <f>_xll.qlSettingsEvaluationDate(Trigger)</f>
-        <v>41796</v>
+        <v>41800</v>
       </c>
       <c r="J18" s="223"/>
     </row>
@@ -2568,7 +2503,7 @@
       </c>
       <c r="I19" s="228">
         <f>[1]!TriggerCounter</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J19" s="223"/>
     </row>
@@ -2608,65 +2543,65 @@
       <c r="E22" s="131"/>
     </row>
     <row r="23" spans="2:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="248" t="s">
+      <c r="B23" s="257" t="s">
         <v>90</v>
       </c>
-      <c r="C23" s="249"/>
-      <c r="D23" s="249"/>
-      <c r="E23" s="250"/>
+      <c r="C23" s="258"/>
+      <c r="D23" s="258"/>
+      <c r="E23" s="259"/>
     </row>
     <row r="24" spans="2:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B24" s="251"/>
-      <c r="C24" s="252"/>
-      <c r="D24" s="252"/>
-      <c r="E24" s="253"/>
+      <c r="B24" s="241"/>
+      <c r="C24" s="242"/>
+      <c r="D24" s="242"/>
+      <c r="E24" s="243"/>
     </row>
     <row r="25" spans="2:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B25" s="251"/>
-      <c r="C25" s="254" t="s">
+      <c r="B25" s="241"/>
+      <c r="C25" s="244" t="s">
         <v>91</v>
       </c>
-      <c r="D25" s="255" t="s">
+      <c r="D25" s="245" t="s">
         <v>92</v>
       </c>
-      <c r="E25" s="253"/>
+      <c r="E25" s="243"/>
     </row>
     <row r="26" spans="2:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B26" s="251"/>
-      <c r="C26" s="254" t="s">
+      <c r="B26" s="241"/>
+      <c r="C26" s="244" t="s">
         <v>93</v>
       </c>
-      <c r="D26" s="256" t="s">
+      <c r="D26" s="246" t="s">
         <v>94</v>
       </c>
-      <c r="E26" s="253"/>
+      <c r="E26" s="243"/>
     </row>
     <row r="27" spans="2:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B27" s="251"/>
-      <c r="C27" s="254" t="s">
+      <c r="B27" s="241"/>
+      <c r="C27" s="244" t="s">
         <v>95</v>
       </c>
-      <c r="D27" s="255" t="s">
+      <c r="D27" s="245" t="s">
         <v>88</v>
       </c>
-      <c r="E27" s="253"/>
+      <c r="E27" s="243"/>
     </row>
     <row r="28" spans="2:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B28" s="251"/>
-      <c r="C28" s="254" t="s">
+      <c r="B28" s="241"/>
+      <c r="C28" s="244" t="s">
         <v>96</v>
       </c>
-      <c r="D28" s="255" t="str">
+      <c r="D28" s="245" t="str">
         <f>D25&amp;"("&amp;D26&amp;","&amp;D27&amp;")"</f>
         <v>JoinHolidays(UnitedKingdom::Exchange,Japan)</v>
       </c>
-      <c r="E28" s="253"/>
+      <c r="E28" s="243"/>
     </row>
     <row r="29" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="257"/>
-      <c r="C29" s="258"/>
-      <c r="D29" s="258"/>
-      <c r="E29" s="259"/>
+      <c r="B29" s="247"/>
+      <c r="C29" s="248"/>
+      <c r="D29" s="248"/>
+      <c r="E29" s="249"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2704,7 +2639,9 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AH50"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2787,7 +2724,7 @@
       </c>
       <c r="B2" s="28" t="str">
         <f>_xll.qlMakeDatedOIS(,E2,F2,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00373#0001</v>
+        <v>obj_003b8#0000</v>
       </c>
       <c r="C2" s="8" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B2,OisEngine)</f>
@@ -2799,11 +2736,11 @@
       </c>
       <c r="E2" s="103">
         <f>SettlementDate</f>
-        <v>41800</v>
+        <v>41802</v>
       </c>
       <c r="F2" s="104">
         <f>_xll.qlCalendarAdvance(Calendar,E2,A3,"mf")</f>
-        <v>41830</v>
+        <v>41834</v>
       </c>
       <c r="G2" s="105">
         <f>_xll.qlQuoteValue($D2,AllTriggers)</f>
@@ -2811,11 +2748,11 @@
       </c>
       <c r="H2" s="106">
         <f>_xll.qlOvernightIndexedSwapFairRate(B2,_xll.ohTrigger(C2,InterestRatesTrigger))</f>
-        <v>6.4109589041194692E-4</v>
+        <v>6.4109589040961534E-4</v>
       </c>
       <c r="I2" s="107">
         <f>G2-H2</f>
-        <v>3.3750410958805312E-4</v>
+        <v>3.375041095903847E-4</v>
       </c>
       <c r="J2" s="108" t="b">
         <v>0</v>
@@ -2829,20 +2766,20 @@
       </c>
       <c r="O2" s="111">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="P2" s="111">
         <f>(O2^2-N2^2)/(O2-N2)</f>
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="Q2" s="108"/>
       <c r="R2" s="122">
         <f>(O2^3-N2^3)/3/(O2-N2)</f>
-        <v>300</v>
+        <v>341.33333333333331</v>
       </c>
       <c r="S2" s="122">
         <f>(O2+N2)/2</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="T2" s="122">
         <v>1</v>
@@ -2855,7 +2792,7 @@
       </c>
       <c r="B3" s="56" t="str">
         <f>_xll.qlMakeDatedOIS(,E3,F3,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00332#0002</v>
+        <v>obj_00375#0001</v>
       </c>
       <c r="C3" s="12" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B3,OisEngine)</f>
@@ -2867,11 +2804,11 @@
       </c>
       <c r="E3" s="96">
         <f>_xll.qlCalendarAdvance(Calendar,_xll.qlLastFixingQuoteReferenceDate(D3),_xll.qlInterestRateIndexFixingDays(A4)&amp;"D","f",,LastFixingsTrigger)</f>
-        <v>41799</v>
+        <v>41802</v>
       </c>
       <c r="F3" s="97">
         <f>F2</f>
-        <v>41830</v>
+        <v>41834</v>
       </c>
       <c r="G3" s="98">
         <f>_xll.qlQuoteValue(D3,AllTriggers)</f>
@@ -2879,11 +2816,11 @@
       </c>
       <c r="H3" s="99">
         <f>_xll.qlOvernightIndexedSwapFairRate(B3,_xll.ohTrigger(C3,InterestRatesTrigger))</f>
-        <v>6.4110549909362515E-4</v>
+        <v>6.4109589040961534E-4</v>
       </c>
       <c r="I3" s="100">
         <f t="shared" ref="I3:I27" si="1">G3-H3</f>
-        <v>3.374945009063749E-4</v>
+        <v>3.375041095903847E-4</v>
       </c>
       <c r="J3" s="108" t="b">
         <f>NOT(ISERROR(I3))</f>
@@ -2900,24 +2837,24 @@
       <c r="M3" s="109"/>
       <c r="N3" s="111">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="O3" s="111">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="P3" s="111">
         <f>(O3^2-N3^2)/(O3-N3)</f>
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="Q3" s="108"/>
       <c r="R3" s="122">
         <f>(O3^3-N3^3)/3/(O3-N3)</f>
-        <v>290.33333333333337</v>
+        <v>341.33333333333331</v>
       </c>
       <c r="S3" s="122">
         <f>(O3+N3)/2</f>
-        <v>14.5</v>
+        <v>16</v>
       </c>
       <c r="T3" s="122">
         <v>1</v>
@@ -2930,7 +2867,7 @@
       </c>
       <c r="B4" s="56" t="str">
         <f>_xll.qlMakeDatedOIS(,E4,F4,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_0037a#0001</v>
+        <v>obj_003bd#0000</v>
       </c>
       <c r="C4" s="12" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B4,OisEngine)</f>
@@ -2941,11 +2878,11 @@
       </c>
       <c r="E4" s="53">
         <f>F3</f>
-        <v>41830</v>
+        <v>41834</v>
       </c>
       <c r="F4" s="54">
         <f>F5</f>
-        <v>41862</v>
+        <v>41863</v>
       </c>
       <c r="G4" s="27" t="e">
         <f>((1+G5*(F5-E5)/360)/(1+G3*(F3-E3)/360)-1)/(F4-E4)*360</f>
@@ -2953,7 +2890,7 @@
       </c>
       <c r="H4" s="15">
         <f>_xll.qlOvernightIndexedSwapFairRate(B4,_xll.ohTrigger(C4,InterestRatesTrigger))</f>
-        <v>6.4106164191307657E-4</v>
+        <v>6.4105935881066253E-4</v>
       </c>
       <c r="I4" s="16" t="e">
         <f>G4-H4</f>
@@ -2974,23 +2911,23 @@
       <c r="M4" s="5"/>
       <c r="N4" s="112">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="O4" s="112">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P4" s="112">
         <f>(O4^2-N4^2)/(O4-N4)</f>
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="R4" s="91">
         <f>(O4^3-N4^3)/3/(O4-N4)</f>
-        <v>2201.3333333333335</v>
+        <v>2232.333333333333</v>
       </c>
       <c r="S4" s="91">
         <f>(O4+N4)/2</f>
-        <v>46</v>
+        <v>46.5</v>
       </c>
       <c r="T4" s="91">
         <v>1</v>
@@ -3006,11 +2943,11 @@
       </c>
       <c r="E5" s="53">
         <f>SettlementDate</f>
-        <v>41800</v>
+        <v>41802</v>
       </c>
       <c r="F5" s="54">
         <f>_xll.qlCalendarAdvance(Calendar,E5,"2M","mf")</f>
-        <v>41862</v>
+        <v>41863</v>
       </c>
       <c r="G5" s="50" t="e">
         <f>_xll.qlQuoteValue(D5,AllTriggers)</f>
@@ -3037,7 +2974,7 @@
       </c>
       <c r="B6" s="28" t="str">
         <f>_xll.qlMakeDatedOIS(,E6,F6,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00379#0001</v>
+        <v>obj_003b7#0000</v>
       </c>
       <c r="C6" s="8" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B6,OisEngine)</f>
@@ -3049,11 +2986,11 @@
       </c>
       <c r="E6" s="103">
         <f>SettlementDate</f>
-        <v>41800</v>
+        <v>41802</v>
       </c>
       <c r="F6" s="104">
         <f>_xll.qlCalendarAdvance(Calendar,E6,A7,"mf")</f>
-        <v>41892</v>
+        <v>41894</v>
       </c>
       <c r="G6" s="105">
         <f>_xll.qlQuoteValue(D6,AllTriggers)</f>
@@ -3061,11 +2998,11 @@
       </c>
       <c r="H6" s="106">
         <f>_xll.qlOvernightIndexedSwapFairRate(B6,_xll.ohTrigger(C6,InterestRatesTrigger))</f>
-        <v>6.4109589041113594E-4</v>
+        <v>6.1643835616455376E-4</v>
       </c>
       <c r="I6" s="107">
         <f t="shared" si="1"/>
-        <v>7.0890410958886413E-4</v>
+        <v>7.3356164383544631E-4</v>
       </c>
       <c r="J6" s="108" t="b">
         <v>0</v>
@@ -3105,7 +3042,7 @@
       </c>
       <c r="B7" s="56" t="str">
         <f>_xll.qlMakeDatedOIS(,E7,F7,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00331#0002</v>
+        <v>obj_00374#0001</v>
       </c>
       <c r="C7" s="12" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B7,OisEngine)</f>
@@ -3117,11 +3054,11 @@
       </c>
       <c r="E7" s="96">
         <f>_xll.qlCalendarAdvance(Calendar,_xll.qlLastFixingQuoteReferenceDate(D7),_xll.qlInterestRateIndexFixingDays(A8)&amp;"D","f",,LastFixingsTrigger)</f>
-        <v>41799</v>
+        <v>41802</v>
       </c>
       <c r="F7" s="97">
         <f>F6</f>
-        <v>41892</v>
+        <v>41894</v>
       </c>
       <c r="G7" s="98">
         <f>_xll.qlQuoteValue(D7,AllTriggers)</f>
@@ -3129,11 +3066,11 @@
       </c>
       <c r="H7" s="99">
         <f>_xll.qlOvernightIndexedSwapFairRate(B7,_xll.ohTrigger(C7,InterestRatesTrigger))</f>
-        <v>6.410998547363853E-4</v>
+        <v>6.1643835616455376E-4</v>
       </c>
       <c r="I7" s="100">
         <f t="shared" si="1"/>
-        <v>7.0890014526361477E-4</v>
+        <v>7.3356164383544631E-4</v>
       </c>
       <c r="J7" s="108" t="b">
         <f>AND(ISERROR(I8),ISERROR(I9),NOT(ISERROR(I7)),E10&lt;&gt;SettlementDate)</f>
@@ -3144,7 +3081,7 @@
       <c r="M7" s="109"/>
       <c r="N7" s="111">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="O7" s="111">
         <f t="shared" si="3"/>
@@ -3152,16 +3089,16 @@
       </c>
       <c r="P7" s="111">
         <f t="shared" ref="P7:P14" si="6">(O7^2-N7^2)/(O7-N7)</f>
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="Q7" s="108"/>
       <c r="R7" s="122">
         <f t="shared" si="4"/>
-        <v>2791</v>
+        <v>2821.333333333333</v>
       </c>
       <c r="S7" s="122">
         <f t="shared" si="5"/>
-        <v>45.5</v>
+        <v>46</v>
       </c>
       <c r="T7" s="122">
         <v>1</v>
@@ -3192,11 +3129,11 @@
       <c r="M8" s="109"/>
       <c r="N8" s="111">
         <f t="shared" si="2"/>
-        <v>-41800</v>
+        <v>-41802</v>
       </c>
       <c r="O8" s="111">
         <f t="shared" si="3"/>
-        <v>-41800</v>
+        <v>-41802</v>
       </c>
       <c r="P8" s="111" t="e">
         <f t="shared" si="6"/>
@@ -3209,7 +3146,7 @@
       </c>
       <c r="S8" s="122">
         <f t="shared" si="5"/>
-        <v>-41800</v>
+        <v>-41802</v>
       </c>
       <c r="T8" s="122">
         <v>1</v>
@@ -3240,20 +3177,20 @@
       </c>
       <c r="K9" s="99">
         <f>AVERAGE(_xll.ohFilter(K10:K12,J10:J12))</f>
-        <v>6.264397388355933E-10</v>
+        <v>1.3454955428348427E-7</v>
       </c>
       <c r="L9" s="99">
         <f>_xll.ohFilter($I$6:$I$9,$J$6:$J$9)-K9*_xll.ohFilter($P$6:$P$9,$J$6:$J$9)</f>
-        <v>7.0884313924738068E-4</v>
+        <v>7.2118308484136573E-4</v>
       </c>
       <c r="M9" s="109"/>
       <c r="N9" s="111">
         <f t="shared" si="2"/>
-        <v>-41800</v>
+        <v>-41802</v>
       </c>
       <c r="O9" s="111">
         <f t="shared" si="3"/>
-        <v>-41800</v>
+        <v>-41802</v>
       </c>
       <c r="P9" s="111" t="e">
         <f t="shared" si="6"/>
@@ -3266,18 +3203,18 @@
       </c>
       <c r="S9" s="122">
         <f t="shared" si="5"/>
-        <v>-41800</v>
+        <v>-41802</v>
       </c>
       <c r="T9" s="122">
         <v>1</v>
       </c>
       <c r="V9" s="82">
         <f t="array" ref="V9:V11">_xll.ohFilter(R6:R14,$J6:$J14)</f>
-        <v>2791</v>
+        <v>2821.333333333333</v>
       </c>
       <c r="W9" s="83">
         <f t="array" ref="W9:W11">_xll.ohFilter(S6:S14,$J6:$J14)</f>
-        <v>45.5</v>
+        <v>46</v>
       </c>
       <c r="X9" s="84">
         <f t="array" ref="X9:X11">_xll.ohFilter(T6:T14,$J6:$J14)</f>
@@ -3285,25 +3222,25 @@
       </c>
       <c r="Z9" s="67">
         <f t="array" ref="Z9:Z11">MMULT(AD9:AF11,AB9:AB11)</f>
-        <v>4.6722025163461978E-10</v>
+        <v>-4.7916534998041182E-13</v>
       </c>
       <c r="AB9" s="67">
         <f t="array" ref="AB9:AB11">_xll.ohFilter(I6:I14,$J6:$J14)</f>
-        <v>7.0890014526361477E-4</v>
+        <v>7.3356164383544631E-4</v>
       </c>
       <c r="AD9" s="73">
         <f t="array" ref="AD9:AF11">MINVERSE(V9:X11)</f>
-        <v>5.2038161318300035E-4</v>
+        <v>5.1229508196721303E-4</v>
       </c>
       <c r="AE9" s="74">
-        <v>-1.0163703382480474E-3</v>
+        <v>-1.0775862068965515E-3</v>
       </c>
       <c r="AF9" s="75">
-        <v>4.9598872506504722E-4</v>
+        <v>5.6529112492933857E-4</v>
       </c>
       <c r="AH9" s="70">
         <f t="array" ref="AH9:AH11">MMULT(V9:X11,Z9:Z11)-AB9:AB11</f>
-        <v>1.0842021724855044E-18</v>
+        <v>-5.4210108624275222E-19</v>
       </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.2">
@@ -3313,7 +3250,7 @@
       </c>
       <c r="B10" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E10,F10,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_0037b#0001</v>
+        <v>obj_003be#0000</v>
       </c>
       <c r="C10" s="12" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B10,OisEngine)</f>
@@ -3337,7 +3274,7 @@
       </c>
       <c r="H10" s="15">
         <f>_xll.qlOvernightIndexedSwapFairRate(B10,_xll.ohTrigger(C10,InterestRatesTrigger))</f>
-        <v>6.4042339973060245E-4</v>
+        <v>6.1364582572549125E-4</v>
       </c>
       <c r="I10" s="16" t="e">
         <f t="shared" si="1"/>
@@ -3358,32 +3295,32 @@
       <c r="M10" s="5"/>
       <c r="N10" s="112">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="O10" s="112">
         <f t="shared" si="3"/>
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="P10" s="112">
         <f t="shared" si="6"/>
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="R10" s="91">
         <f t="shared" si="4"/>
-        <v>3621.3333333333335</v>
+        <v>3409.3333333333335</v>
       </c>
       <c r="S10" s="91">
         <f t="shared" si="5"/>
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="T10" s="91">
         <v>1</v>
       </c>
       <c r="V10" s="85">
-        <v>6481.333333333333</v>
+        <v>6789.333333333333</v>
       </c>
       <c r="W10" s="86">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="X10" s="87">
         <v>1</v>
@@ -3392,25 +3329,25 @@
         <v>46</v>
       </c>
       <c r="Z10" s="68">
-        <v>-5.5278217853959341E-8</v>
+        <v>2.6915852507036314E-7</v>
       </c>
       <c r="AA10" s="58" t="s">
         <v>47</v>
       </c>
       <c r="AB10" s="68">
-        <v>7.0893835808768374E-4</v>
+        <v>7.421728153095893E-4</v>
       </c>
       <c r="AD10" s="76">
-        <v>-9.5750216825672071E-2</v>
+        <v>-9.4774590163934413E-2</v>
       </c>
       <c r="AE10" s="77">
-        <v>0.15576214223764079</v>
+        <v>0.16487068965517238</v>
       </c>
       <c r="AF10" s="78">
-        <v>-6.001192541196871E-2</v>
+        <v>-7.0096099491237976E-2</v>
       </c>
       <c r="AH10" s="71">
-        <v>1.951563910473908E-18</v>
+        <v>-6.5052130349130266E-19</v>
       </c>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.2">
@@ -3420,7 +3357,7 @@
       </c>
       <c r="B11" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E11,F11,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_0037c#0001</v>
+        <v>obj_003bf#0000</v>
       </c>
       <c r="C11" s="12" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B11,OisEngine)</f>
@@ -3444,7 +3381,7 @@
       </c>
       <c r="H11" s="15">
         <f>_xll.qlOvernightIndexedSwapFairRate(B11,_xll.ohTrigger(C11,InterestRatesTrigger))</f>
-        <v>6.4285295262164635E-4</v>
+        <v>6.0717889088916007E-4</v>
       </c>
       <c r="I11" s="16" t="e">
         <f t="shared" si="1"/>
@@ -3465,53 +3402,53 @@
       <c r="M11" s="5"/>
       <c r="N11" s="112">
         <f t="shared" si="2"/>
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="O11" s="112">
         <f t="shared" si="3"/>
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="P11" s="112">
         <f t="shared" si="6"/>
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="R11" s="91">
         <f t="shared" si="4"/>
-        <v>7429.333333333333</v>
+        <v>7105.333333333333</v>
       </c>
       <c r="S11" s="91">
         <f t="shared" si="5"/>
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="T11" s="91">
         <v>1</v>
       </c>
       <c r="V11" s="88">
-        <v>12369.333333333334</v>
+        <v>12154.333333333334</v>
       </c>
       <c r="W11" s="89">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="X11" s="90">
         <v>1</v>
       </c>
       <c r="Z11" s="69">
-        <v>7.1011129245365876E-4</v>
+        <v>7.2118170356738317E-4</v>
       </c>
       <c r="AB11" s="69">
-        <v>7.0992044795798045E-4</v>
+        <v>7.499758418145271E-4</v>
       </c>
       <c r="AD11" s="79">
-        <v>3.9042497831743255</v>
+        <v>3.9142759562841527</v>
       </c>
       <c r="AE11" s="80">
-        <v>-4.250487857762355</v>
+        <v>-4.5438218390804597</v>
       </c>
       <c r="AF11" s="81">
-        <v>1.3462380745880296</v>
+        <v>1.6295458827963067</v>
       </c>
       <c r="AH11" s="72">
-        <v>3.1441863002079629E-18</v>
+        <v>-5.4210108624275222E-19</v>
       </c>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.2">
@@ -3520,7 +3457,7 @@
       </c>
       <c r="B12" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E12,F12,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00375#0001</v>
+        <v>obj_003bc#0000</v>
       </c>
       <c r="C12" s="12" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B12,OisEngine)</f>
@@ -3532,11 +3469,11 @@
       </c>
       <c r="E12" s="53">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,A12&amp;"M","mf")</f>
-        <v>41830</v>
+        <v>41834</v>
       </c>
       <c r="F12" s="54">
         <f>_xll.qlInterestRateIndexMaturity($A$8,E12)</f>
-        <v>41922</v>
+        <v>41926</v>
       </c>
       <c r="G12" s="50">
         <f>_xll.qlQuoteValue(D12,AllTriggers)</f>
@@ -3544,11 +3481,11 @@
       </c>
       <c r="H12" s="15">
         <f>_xll.qlOvernightIndexedSwapFairRate(B12,_xll.ohTrigger(C12,InterestRatesTrigger))</f>
-        <v>6.4106164191231633E-4</v>
+        <v>6.0782718469041077E-4</v>
       </c>
       <c r="I12" s="16">
         <f>G12-H12</f>
-        <v>7.0893835808768374E-4</v>
+        <v>7.421728153095893E-4</v>
       </c>
       <c r="J12" s="1" t="b">
         <f>AND(NOT(ISERROR(I12)),E12&lt;&gt;$E$11,E12&lt;&gt;$E$10)</f>
@@ -3556,32 +3493,32 @@
       </c>
       <c r="K12" s="15">
         <f>(I12-_xll.ohFilter($I$6:$I$9,$J$6:$J$9))/(P12-_xll.ohFilter($P$6:$P$9,$J$6:$J$9))</f>
-        <v>6.264397388355933E-10</v>
+        <v>1.3454955428348427E-7</v>
       </c>
       <c r="L12" s="15">
         <f>_xll.ohFilter($I$6:$I$9,$J$6:$J$9)-K12*_xll.ohFilter($P$6:$P$9,$J$6:$J$9)</f>
-        <v>7.0884313924738068E-4</v>
+        <v>7.2118308484136573E-4</v>
       </c>
       <c r="M12" s="5"/>
       <c r="N12" s="112">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="O12" s="112">
         <f t="shared" si="3"/>
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="P12" s="112">
         <f t="shared" si="6"/>
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="R12" s="91">
         <f t="shared" si="4"/>
-        <v>6481.333333333333</v>
+        <v>6789.333333333333</v>
       </c>
       <c r="S12" s="91">
         <f t="shared" si="5"/>
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="T12" s="91">
         <v>1</v>
@@ -3596,7 +3533,7 @@
       </c>
       <c r="B13" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E13,F13,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00370#0001</v>
+        <v>obj_003b3#0000</v>
       </c>
       <c r="C13" s="12" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B13,OisEngine)</f>
@@ -3608,11 +3545,11 @@
       </c>
       <c r="E13" s="53">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,A13&amp;"M","mf")</f>
-        <v>41862</v>
+        <v>41863</v>
       </c>
       <c r="F13" s="54">
         <f>_xll.qlInterestRateIndexMaturity($A$8,E13)</f>
-        <v>41954</v>
+        <v>41955</v>
       </c>
       <c r="G13" s="50">
         <f>_xll.qlQuoteValue(D13,AllTriggers)</f>
@@ -3620,11 +3557,11 @@
       </c>
       <c r="H13" s="15">
         <f>_xll.qlOvernightIndexedSwapFairRate(B13,_xll.ohTrigger(C13,InterestRatesTrigger))</f>
-        <v>6.4007955204201962E-4</v>
+        <v>6.0002415818547297E-4</v>
       </c>
       <c r="I13" s="16">
         <f>G13-H13</f>
-        <v>7.0992044795798045E-4</v>
+        <v>7.499758418145271E-4</v>
       </c>
       <c r="J13" s="1" t="b">
         <f>AND(NOT(ISERROR(I13)),E13&lt;&gt;$E$11,E13&lt;&gt;$E$10)</f>
@@ -3632,32 +3569,32 @@
       </c>
       <c r="K13" s="15">
         <f>(I13-_xll.ohFilter($I$6:$I$9,$J$6:$J$9))/(P13-_xll.ohFilter($P$6:$P$9,$J$6:$J$9))</f>
-        <v>8.1624215549254421E-9</v>
+        <v>1.3454260638590817E-7</v>
       </c>
       <c r="L13" s="15">
         <f>_xll.ohFilter($I$6:$I$9,$J$6:$J$9)-K13*_xll.ohFilter($P$6:$P$9,$J$6:$J$9)</f>
-        <v>7.081573649021165E-4</v>
+        <v>7.2118372404794272E-4</v>
       </c>
       <c r="M13" s="5"/>
       <c r="N13" s="112">
         <f t="shared" si="2"/>
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O13" s="112">
         <f t="shared" si="3"/>
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="P13" s="112">
         <f t="shared" si="6"/>
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="R13" s="91">
         <f t="shared" si="4"/>
-        <v>12369.333333333334</v>
+        <v>12154.333333333334</v>
       </c>
       <c r="S13" s="91">
         <f t="shared" si="5"/>
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="T13" s="91">
         <v>1</v>
@@ -3672,7 +3609,7 @@
       </c>
       <c r="B14" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E14,F14,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00378#0001</v>
+        <v>obj_003b5#0000</v>
       </c>
       <c r="C14" s="12" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B14,OisEngine)</f>
@@ -3684,11 +3621,11 @@
       </c>
       <c r="E14" s="53">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,A14&amp;"M","mf")</f>
-        <v>41892</v>
+        <v>41894</v>
       </c>
       <c r="F14" s="54">
         <f>_xll.qlInterestRateIndexMaturity($A$8,E14)</f>
-        <v>41983</v>
+        <v>41985</v>
       </c>
       <c r="G14" s="50">
         <f>_xll.qlQuoteValue(D14,AllTriggers)</f>
@@ -3696,11 +3633,11 @@
       </c>
       <c r="H14" s="15">
         <f>_xll.qlOvernightIndexedSwapFairRate(B14,_xll.ohTrigger(C14,InterestRatesTrigger))</f>
-        <v>5.9141296549541987E-4</v>
+        <v>6.16341261308051E-4</v>
       </c>
       <c r="I14" s="16">
         <f>G14-H14</f>
-        <v>7.585870345045802E-4</v>
+        <v>7.3365873869194907E-4</v>
       </c>
       <c r="J14" s="1" t="b">
         <f>AND(NOT(ISERROR(I14)),E14&lt;&gt;$E$11,E14&lt;&gt;$E$10)</f>
@@ -3708,11 +3645,11 @@
       </c>
       <c r="K14" s="15">
         <f>(I14-_xll.ohFilter($I$6:$I$9,$J$6:$J$9))/(P14-_xll.ohFilter($P$6:$P$9,$J$6:$J$9))</f>
-        <v>2.7003744152698603E-7</v>
+        <v>5.3057298635388944E-10</v>
       </c>
       <c r="L14" s="15">
         <f>_xll.ohFilter($I$6:$I$9,$J$6:$J$9)-K14*_xll.ohFilter($P$6:$P$9,$J$6:$J$9)</f>
-        <v>6.84326738084659E-4</v>
+        <v>7.3351283112070174E-4</v>
       </c>
       <c r="M14" s="5"/>
       <c r="N14" s="112">
@@ -3748,7 +3685,7 @@
       </c>
       <c r="B15" s="28" t="str">
         <f>_xll.qlMakeDatedOIS(,E15,F15,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00377#0001</v>
+        <v>obj_003b1#0000</v>
       </c>
       <c r="C15" s="8" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B15,OisEngine)</f>
@@ -3760,11 +3697,11 @@
       </c>
       <c r="E15" s="103">
         <f>SettlementDate</f>
-        <v>41800</v>
+        <v>41802</v>
       </c>
       <c r="F15" s="104">
         <f>_xll.qlCalendarAdvance(Calendar,E15,A16,"mf")</f>
-        <v>41983</v>
+        <v>41985</v>
       </c>
       <c r="G15" s="105">
         <f>_xll.qlQuoteValue($D15,AllTriggers)</f>
@@ -3816,7 +3753,7 @@
       </c>
       <c r="B16" s="56" t="str">
         <f>_xll.qlMakeDatedOIS(,E16,F16,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00333#0002</v>
+        <v>obj_00376#0001</v>
       </c>
       <c r="C16" s="12" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B16,OisEngine)</f>
@@ -3828,11 +3765,11 @@
       </c>
       <c r="E16" s="96">
         <f>_xll.qlCalendarAdvance(Calendar,_xll.qlLastFixingQuoteReferenceDate(D16),_xll.qlInterestRateIndexFixingDays(A17)&amp;"D","f",,LastFixingsTrigger)</f>
-        <v>41799</v>
+        <v>41802</v>
       </c>
       <c r="F16" s="97">
         <f>_xll.qlInterestRateIndexMaturity(A17,E16)</f>
-        <v>41982</v>
+        <v>41985</v>
       </c>
       <c r="G16" s="98">
         <f>_xll.qlQuoteValue(D16,AllTriggers)</f>
@@ -3840,11 +3777,11 @@
       </c>
       <c r="H16" s="99">
         <f>_xll.qlOvernightIndexedSwapFairRate(B16,_xll.ohTrigger(C16,InterestRatesTrigger))</f>
-        <v>6.1726123800877211E-4</v>
+        <v>6.1643835616435915E-4</v>
       </c>
       <c r="I16" s="100">
         <f t="shared" si="1"/>
-        <v>1.2006387619912279E-3</v>
+        <v>1.2014616438356411E-3</v>
       </c>
       <c r="J16" s="108" t="b">
         <f>AND(NOT(ISERROR(I16)))</f>
@@ -3855,24 +3792,24 @@
       <c r="M16" s="109"/>
       <c r="N16" s="111">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="O16" s="111">
         <f t="shared" si="3"/>
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="P16" s="111">
         <f t="shared" si="7"/>
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="Q16" s="108"/>
       <c r="R16" s="122">
         <f t="shared" si="8"/>
-        <v>10981</v>
+        <v>11163</v>
       </c>
       <c r="S16" s="122">
         <f t="shared" si="9"/>
-        <v>90.5</v>
+        <v>91.5</v>
       </c>
       <c r="T16" s="122">
         <v>1</v>
@@ -3903,11 +3840,11 @@
       <c r="M17" s="109"/>
       <c r="N17" s="111">
         <f t="shared" si="2"/>
-        <v>-41800</v>
+        <v>-41802</v>
       </c>
       <c r="O17" s="111">
         <f t="shared" si="3"/>
-        <v>-41800</v>
+        <v>-41802</v>
       </c>
       <c r="P17" s="111" t="e">
         <f t="shared" si="7"/>
@@ -3920,7 +3857,7 @@
       </c>
       <c r="S17" s="122">
         <f t="shared" si="9"/>
-        <v>-41800</v>
+        <v>-41802</v>
       </c>
       <c r="T17" s="122">
         <v>1</v>
@@ -3951,20 +3888,20 @@
       </c>
       <c r="K18" s="99">
         <f>AVERAGE(_xll.ohFilter(K19:K21,J19:J21))</f>
-        <v>-3.331718970181937E-8</v>
+        <v>-1.5723874883343609E-7</v>
       </c>
       <c r="L18" s="99">
         <f>_xll.ohFilter($I$15:$I$18,$J$15:$J$18)-K18*_xll.ohFilter($P$15:$P$18,$J$15:$J$18)</f>
-        <v>1.2066691733272571E-3</v>
+        <v>1.23023633487216E-3</v>
       </c>
       <c r="M18" s="109"/>
       <c r="N18" s="111">
         <f t="shared" si="2"/>
-        <v>-41800</v>
+        <v>-41802</v>
       </c>
       <c r="O18" s="111">
         <f t="shared" si="3"/>
-        <v>-41800</v>
+        <v>-41802</v>
       </c>
       <c r="P18" s="111" t="e">
         <f t="shared" si="7"/>
@@ -3977,18 +3914,18 @@
       </c>
       <c r="S18" s="122">
         <f t="shared" si="9"/>
-        <v>-41800</v>
+        <v>-41802</v>
       </c>
       <c r="T18" s="122">
         <v>1</v>
       </c>
       <c r="V18" s="82">
         <f t="array" ref="V18:V20">_xll.ohFilter(R15:R24,$J15:$J24)</f>
-        <v>10981</v>
+        <v>11163</v>
       </c>
       <c r="W18" s="83">
         <f t="array" ref="W18:W20">_xll.ohFilter(S15:S24,$J15:$J24)</f>
-        <v>90.5</v>
+        <v>91.5</v>
       </c>
       <c r="X18" s="84">
         <f t="array" ref="X18:X20">_xll.ohFilter(T15:T24,$J15:$J24)</f>
@@ -3996,25 +3933,25 @@
       </c>
       <c r="Z18" s="67">
         <f t="array" ref="Z18:Z20">MMULT(AD18:AF20,AB18:AB20)</f>
-        <v>1.7017064290611148E-9</v>
+        <v>9.9010787776119224E-9</v>
       </c>
       <c r="AB18" s="67">
         <f t="array" ref="AB18:AB20">_xll.ohFilter(I15:I24,$J15:$J24)</f>
-        <v>1.2006387619912279E-3</v>
+        <v>1.2014616438356411E-3</v>
       </c>
       <c r="AD18" s="73">
         <f t="array" ref="AD18:AF20">MINVERSE(V18:X20)</f>
-        <v>5.201109570041612E-4</v>
+        <v>5.0808705224828562E-4</v>
       </c>
       <c r="AE18" s="74">
-        <v>-1.073777459621494E-3</v>
+        <v>-1.0774949556299855E-3</v>
       </c>
       <c r="AF18" s="75">
-        <v>5.5366650261733281E-4</v>
+        <v>5.694079033816996E-4</v>
       </c>
       <c r="AH18" s="70">
         <f t="array" ref="AH18:AH20">MMULT(V18:X20,Z18:Z20)-AB18:AB20</f>
-        <v>1.0842021724855044E-18</v>
+        <v>-3.2526065174565133E-18</v>
       </c>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.2">
@@ -4023,7 +3960,7 @@
       </c>
       <c r="B19" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E19,F19,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00372#0001</v>
+        <v>obj_003b6#0000</v>
       </c>
       <c r="C19" s="12" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B19,OisEngine)</f>
@@ -4035,11 +3972,11 @@
       </c>
       <c r="E19" s="53">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,A19&amp;"M","mf")</f>
-        <v>41830</v>
+        <v>41834</v>
       </c>
       <c r="F19" s="54">
         <f>_xll.qlInterestRateIndexMaturity($A$17,E19)</f>
-        <v>42017</v>
+        <v>42018</v>
       </c>
       <c r="G19" s="27">
         <f>_xll.qlQuoteValue(D19,AllTriggers)</f>
@@ -4047,11 +3984,11 @@
       </c>
       <c r="H19" s="15">
         <f>_xll.qlOvernightIndexedSwapFairRate(B19,_xll.ohTrigger(C19,InterestRatesTrigger))</f>
-        <v>6.0265481653182793E-4</v>
+        <v>6.1528453359098153E-4</v>
       </c>
       <c r="I19" s="16">
         <f t="shared" ref="I19:I24" si="11">G19-H19</f>
-        <v>1.1973451834681719E-3</v>
+        <v>1.1847154664090184E-3</v>
       </c>
       <c r="J19" s="1" t="b">
         <f t="shared" ref="J19:J24" si="12">NOT(ISERROR(I19))</f>
@@ -4059,41 +3996,41 @@
       </c>
       <c r="K19" s="15">
         <f>(I19-_xll.ohFilter($I$15:$I$18,$J$15:$J$18))/(P19-_xll.ohFilter($P$15:$P$18,$J$15:$J$18))</f>
-        <v>-4.9902704894787611E-8</v>
+        <v>-2.5763349887111764E-7</v>
       </c>
       <c r="L19" s="15">
         <f>_xll.ohFilter($I$15:$I$18,$J$15:$J$18)-K19*_xll.ohFilter($P$15:$P$18,$J$15:$J$18)</f>
-        <v>1.2096711515771845E-3</v>
+        <v>1.2486085741290555E-3</v>
       </c>
       <c r="M19" s="5"/>
       <c r="N19" s="112">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="O19" s="112">
         <f t="shared" si="3"/>
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="P19" s="112">
         <f t="shared" si="7"/>
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="R19" s="91">
         <f t="shared" si="8"/>
-        <v>18166.333333333336</v>
+        <v>18197.333333333336</v>
       </c>
       <c r="S19" s="91">
         <f t="shared" si="9"/>
-        <v>123.5</v>
+        <v>124</v>
       </c>
       <c r="T19" s="91">
         <v>1</v>
       </c>
       <c r="V19" s="85">
-        <v>18166.333333333336</v>
+        <v>18197.333333333336</v>
       </c>
       <c r="W19" s="86">
-        <v>123.5</v>
+        <v>124</v>
       </c>
       <c r="X19" s="87">
         <v>1</v>
@@ -4102,25 +4039,25 @@
         <v>46</v>
       </c>
       <c r="Z19" s="68">
-        <v>-4.7033049852535764E-7</v>
+        <v>-2.6582666433212201E-6</v>
       </c>
       <c r="AA19" s="58" t="s">
         <v>47</v>
       </c>
       <c r="AB19" s="68">
-        <v>1.1973451834681719E-3</v>
+        <v>1.1847154664090184E-3</v>
       </c>
       <c r="AD19" s="76">
-        <v>-0.14355062413314851</v>
+        <v>-0.1407401134727751</v>
       </c>
       <c r="AE19" s="77">
-        <v>0.26410451433940335</v>
+        <v>0.26398334408881624</v>
       </c>
       <c r="AF19" s="78">
-        <v>-0.12055389020625484</v>
+        <v>-0.1232432306160411</v>
       </c>
       <c r="AH19" s="71">
-        <v>6.5052130349130266E-19</v>
+        <v>-5.4210108624275222E-18</v>
       </c>
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.2">
@@ -4129,7 +4066,7 @@
       </c>
       <c r="B20" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E20,F20,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_0036f#0001</v>
+        <v>obj_003b2#0000</v>
       </c>
       <c r="C20" s="12" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B20,OisEngine)</f>
@@ -4141,7 +4078,7 @@
       </c>
       <c r="E20" s="53">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,A20&amp;"M","mf")</f>
-        <v>41862</v>
+        <v>41863</v>
       </c>
       <c r="F20" s="54">
         <f>_xll.qlInterestRateIndexMaturity($A$17,E20)</f>
@@ -4153,11 +4090,11 @@
       </c>
       <c r="H20" s="15">
         <f>_xll.qlOvernightIndexedSwapFairRate(B20,_xll.ohTrigger(C20,InterestRatesTrigger))</f>
-        <v>6.0267526177906696E-4</v>
+        <v>6.1283890042673761E-4</v>
       </c>
       <c r="I20" s="16">
         <f t="shared" si="11"/>
-        <v>1.197324738220933E-3</v>
+        <v>1.1871610995732623E-3</v>
       </c>
       <c r="J20" s="1" t="b">
         <f t="shared" si="12"/>
@@ -4165,62 +4102,62 @@
       </c>
       <c r="K20" s="15">
         <f>(I20-_xll.ohFilter($I$15:$I$18,$J$15:$J$18))/(P20-_xll.ohFilter($P$15:$P$18,$J$15:$J$18))</f>
-        <v>-2.5890810705428893E-8</v>
+        <v>-1.1626458749901408E-7</v>
       </c>
       <c r="L20" s="15">
         <f>_xll.ohFilter($I$15:$I$18,$J$15:$J$18)-K20*_xll.ohFilter($P$15:$P$18,$J$15:$J$18)</f>
-        <v>1.2053249987289106E-3</v>
+        <v>1.2227380633479607E-3</v>
       </c>
       <c r="M20" s="5"/>
       <c r="N20" s="112">
         <f t="shared" si="2"/>
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O20" s="112">
         <f t="shared" si="3"/>
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="P20" s="112">
         <f t="shared" si="7"/>
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="R20" s="91">
         <f t="shared" si="8"/>
-        <v>26722.333333333336</v>
+        <v>26230.333333333332</v>
       </c>
       <c r="S20" s="91">
         <f t="shared" si="9"/>
-        <v>154.5</v>
+        <v>153</v>
       </c>
       <c r="T20" s="91">
         <v>1</v>
       </c>
       <c r="V20" s="88">
-        <v>26722.333333333336</v>
+        <v>26230.333333333332</v>
       </c>
       <c r="W20" s="89">
-        <v>154.5</v>
+        <v>153</v>
       </c>
       <c r="X20" s="90">
         <v>1</v>
       </c>
       <c r="Z20" s="69">
-        <v>1.2245172338102538E-3</v>
+        <v>1.3341672993050476E-3</v>
       </c>
       <c r="AB20" s="69">
-        <v>1.197324738220933E-3</v>
+        <v>1.1871610995732623E-3</v>
       </c>
       <c r="AD20" s="79">
-        <v>8.2799930651872469</v>
+        <v>8.2059446185113085</v>
       </c>
       <c r="AE20" s="80">
-        <v>-12.110308263612378</v>
+        <v>-12.126399794429158</v>
       </c>
       <c r="AF20" s="81">
-        <v>4.830315198425132</v>
+        <v>4.9204551759178488</v>
       </c>
       <c r="AH20" s="72">
-        <v>4.3368086899420177E-19</v>
+        <v>-8.2399365108898337E-18</v>
       </c>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.2">
@@ -4229,7 +4166,7 @@
       </c>
       <c r="B21" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E21,F21,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00376#0001</v>
+        <v>obj_003b0#0000</v>
       </c>
       <c r="C21" s="12" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B21,OisEngine)</f>
@@ -4241,11 +4178,11 @@
       </c>
       <c r="E21" s="53">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,A21&amp;"M","mf")</f>
-        <v>41892</v>
+        <v>41894</v>
       </c>
       <c r="F21" s="54">
         <f>_xll.qlInterestRateIndexMaturity($A$17,E21)</f>
-        <v>42073</v>
+        <v>42075</v>
       </c>
       <c r="G21" s="27">
         <f>_xll.qlQuoteValue(D21,AllTriggers)</f>
@@ -4253,11 +4190,11 @@
       </c>
       <c r="H21" s="15">
         <f>_xll.qlOvernightIndexedSwapFairRate(B21,_xll.ohTrigger(C21,InterestRatesTrigger))</f>
-        <v>6.038063198537364E-4</v>
+        <v>6.1634126130805111E-4</v>
       </c>
       <c r="I21" s="16">
         <f t="shared" si="11"/>
-        <v>1.1961936801462634E-3</v>
+        <v>1.1836587386919489E-3</v>
       </c>
       <c r="J21" s="1" t="b">
         <f t="shared" si="12"/>
@@ -4265,11 +4202,11 @@
       </c>
       <c r="K21" s="15">
         <f>(I21-_xll.ohFilter($I$15:$I$18,$J$15:$J$18))/(P21-_xll.ohFilter($P$15:$P$18,$J$15:$J$18))</f>
-        <v>-2.4158053505241608E-8</v>
+        <v>-9.7818160130176517E-8</v>
       </c>
       <c r="L21" s="15">
         <f>_xll.ohFilter($I$15:$I$18,$J$15:$J$18)-K21*_xll.ohFilter($P$15:$P$18,$J$15:$J$18)</f>
-        <v>1.2050113696756765E-3</v>
+        <v>1.2193623671394635E-3</v>
       </c>
       <c r="M21" s="5"/>
       <c r="N21" s="112">
@@ -4306,7 +4243,7 @@
       </c>
       <c r="B22" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E22,F22,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_0036d#0001</v>
+        <v>obj_003bb#0000</v>
       </c>
       <c r="C22" s="12" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B22,OisEngine)</f>
@@ -4318,11 +4255,11 @@
       </c>
       <c r="E22" s="53">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,A22&amp;"M","mf")</f>
-        <v>41922</v>
+        <v>41926</v>
       </c>
       <c r="F22" s="54">
         <f>_xll.qlInterestRateIndexMaturity($A$17,E22)</f>
-        <v>42104</v>
+        <v>42108</v>
       </c>
       <c r="G22" s="27">
         <f>_xll.qlQuoteValue(D22,AllTriggers)</f>
@@ -4330,11 +4267,11 @@
       </c>
       <c r="H22" s="15">
         <f>_xll.qlOvernightIndexedSwapFairRate(B22,_xll.ohTrigger(C22,InterestRatesTrigger))</f>
-        <v>6.0103710904389697E-4</v>
+        <v>5.998067238031726E-4</v>
       </c>
       <c r="I22" s="16">
         <f t="shared" si="11"/>
-        <v>1.198962890956103E-3</v>
+        <v>1.2001932761968274E-3</v>
       </c>
       <c r="J22" s="1" t="b">
         <f t="shared" si="12"/>
@@ -4342,32 +4279,32 @@
       </c>
       <c r="K22" s="15">
         <f>(I22-_xll.ohFilter($I$15:$I$18,$J$15:$J$18))/(P22-_xll.ohFilter($P$15:$P$18,$J$15:$J$18))</f>
-        <v>-6.8402899392853634E-9</v>
+        <v>-5.1350916551162829E-9</v>
       </c>
       <c r="L22" s="15">
         <f>_xll.ohFilter($I$15:$I$18,$J$15:$J$18)-K22*_xll.ohFilter($P$15:$P$18,$J$15:$J$18)</f>
-        <v>1.2018768544702386E-3</v>
+        <v>1.2024013656085273E-3</v>
       </c>
       <c r="M22" s="5"/>
       <c r="N22" s="112">
         <f t="shared" si="2"/>
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="O22" s="112">
         <f t="shared" si="3"/>
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="P22" s="112">
         <f t="shared" si="7"/>
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="R22" s="91">
         <f t="shared" si="8"/>
-        <v>48129.333333333328</v>
+        <v>48985.333333333328</v>
       </c>
       <c r="S22" s="91">
         <f t="shared" si="9"/>
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="T22" s="91">
         <v>1</v>
@@ -4383,7 +4320,7 @@
       </c>
       <c r="B23" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E23,F23,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_0036c#0001</v>
+        <v>obj_003b9#0000</v>
       </c>
       <c r="C23" s="12" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B23,OisEngine)</f>
@@ -4395,23 +4332,23 @@
       </c>
       <c r="E23" s="53">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,A23&amp;"M","mf")</f>
-        <v>41953</v>
+        <v>41955</v>
       </c>
       <c r="F23" s="54">
         <f>_xll.qlInterestRateIndexMaturity($A$17,E23)</f>
-        <v>42135</v>
+        <v>42136</v>
       </c>
       <c r="G23" s="27">
         <f>_xll.qlQuoteValue(D23,AllTriggers)</f>
-        <v>1.8E-3</v>
+        <v>1.7499999999999998E-3</v>
       </c>
       <c r="H23" s="15">
         <f>_xll.qlOvernightIndexedSwapFairRate(B23,_xll.ohTrigger(C23,InterestRatesTrigger))</f>
-        <v>5.9508603563005976E-4</v>
+        <v>5.8190702791322089E-4</v>
       </c>
       <c r="I23" s="16">
         <f t="shared" si="11"/>
-        <v>1.2049139643699402E-3</v>
+        <v>1.168092972086779E-3</v>
       </c>
       <c r="J23" s="1" t="b">
         <f t="shared" si="12"/>
@@ -4419,11 +4356,11 @@
       </c>
       <c r="K23" s="15">
         <f>(I23-_xll.ohFilter($I$15:$I$18,$J$15:$J$18))/(P23-_xll.ohFilter($P$15:$P$18,$J$15:$J$18))</f>
-        <v>1.3925740647271317E-8</v>
+        <v>-1.0976536759494089E-7</v>
       </c>
       <c r="L23" s="15">
         <f>_xll.ohFilter($I$15:$I$18,$J$15:$J$18)-K23*_xll.ohFilter($P$15:$P$18,$J$15:$J$18)</f>
-        <v>1.1981182029340719E-3</v>
+        <v>1.2215487061055152E-3</v>
       </c>
       <c r="M23" s="5"/>
       <c r="N23" s="112">
@@ -4432,19 +4369,19 @@
       </c>
       <c r="O23" s="112">
         <f t="shared" si="3"/>
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="P23" s="112">
         <f t="shared" si="7"/>
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="R23" s="91">
         <f t="shared" si="8"/>
-        <v>62296.333333333328</v>
+        <v>62022.333333333336</v>
       </c>
       <c r="S23" s="91">
         <f t="shared" si="9"/>
-        <v>244</v>
+        <v>243.5</v>
       </c>
       <c r="T23" s="91">
         <v>1</v>
@@ -4460,7 +4397,7 @@
       </c>
       <c r="B24" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E24,F24,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00374#0001</v>
+        <v>obj_003ba#0000</v>
       </c>
       <c r="C24" s="12" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B24,OisEngine)</f>
@@ -4472,23 +4409,23 @@
       </c>
       <c r="E24" s="53">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,A24&amp;"M","mf")</f>
-        <v>41983</v>
+        <v>41985</v>
       </c>
       <c r="F24" s="54">
         <f>_xll.qlInterestRateIndexMaturity($A$17,E24)</f>
-        <v>42165</v>
+        <v>42167</v>
       </c>
       <c r="G24" s="27">
         <f>_xll.qlQuoteValue(D24,AllTriggers)</f>
-        <v>1.8E-3</v>
+        <v>1.7499999999999998E-3</v>
       </c>
       <c r="H24" s="15">
         <f>_xll.qlOvernightIndexedSwapFairRate(B24,_xll.ohTrigger(C24,InterestRatesTrigger))</f>
-        <v>6.1624525191640524E-4</v>
+        <v>5.6681019324561922E-4</v>
       </c>
       <c r="I24" s="16">
         <f t="shared" si="11"/>
-        <v>1.1837547480835946E-3</v>
+        <v>1.1831898067543806E-3</v>
       </c>
       <c r="J24" s="1" t="b">
         <f t="shared" si="12"/>
@@ -4496,11 +4433,11 @@
       </c>
       <c r="K24" s="15">
         <f>(I24-_xll.ohFilter($I$15:$I$18,$J$15:$J$18))/(P24-_xll.ohFilter($P$15:$P$18,$J$15:$J$18))</f>
-        <v>-4.6005487486739205E-8</v>
+        <v>-5.0059827619891699E-8</v>
       </c>
       <c r="L24" s="15">
         <f>_xll.ohFilter($I$15:$I$18,$J$15:$J$18)-K24*_xll.ohFilter($P$15:$P$18,$J$15:$J$18)</f>
-        <v>1.2089657552263277E-3</v>
+        <v>1.2106225922900813E-3</v>
       </c>
       <c r="M24" s="5"/>
       <c r="N24" s="112">
@@ -4533,7 +4470,7 @@
       </c>
       <c r="B25" s="28" t="str">
         <f>_xll.qlMakeDatedOIS(,E25,F25,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_0036e#0001</v>
+        <v>obj_003af#0000</v>
       </c>
       <c r="C25" s="8" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B25,OisEngine)</f>
@@ -4545,23 +4482,23 @@
       </c>
       <c r="E25" s="103">
         <f>SettlementDate</f>
-        <v>41800</v>
+        <v>41802</v>
       </c>
       <c r="F25" s="104">
         <f>_xll.qlCalendarAdvance(Calendar,E25,A26,"mf")</f>
-        <v>42165</v>
+        <v>42167</v>
       </c>
       <c r="G25" s="105">
         <f>_xll.qlQuoteValue($D25,AllTriggers)</f>
-        <v>3.3571E-3</v>
+        <v>3.3356999999999996E-3</v>
       </c>
       <c r="H25" s="106">
         <f>_xll.qlOvernightIndexedSwapFairRate(B25,_xll.ohTrigger(C25,InterestRatesTrigger))</f>
-        <v>6.1643835616447993E-4</v>
+        <v>5.9178082191774304E-4</v>
       </c>
       <c r="I25" s="107">
         <f t="shared" si="1"/>
-        <v>2.7406616438355202E-3</v>
+        <v>2.7439191780822565E-3</v>
       </c>
       <c r="J25" s="108" t="b">
         <v>0</v>
@@ -4601,7 +4538,7 @@
       </c>
       <c r="B26" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E26,F26,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00334#0002</v>
+        <v>obj_00377#0001</v>
       </c>
       <c r="C26" s="12" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B26,OisEngine)</f>
@@ -4613,23 +4550,23 @@
       </c>
       <c r="E26" s="96">
         <f>_xll.qlCalendarAdvance(Calendar,_xll.qlLastFixingQuoteReferenceDate(D26),_xll.qlInterestRateIndexFixingDays(A27)&amp;"D","f",,LastFixingsTrigger)</f>
-        <v>41799</v>
+        <v>41802</v>
       </c>
       <c r="F26" s="97">
         <f>_xll.qlInterestRateIndexMaturity(A27,E26)</f>
-        <v>42164</v>
+        <v>42167</v>
       </c>
       <c r="G26" s="98">
         <f>_xll.qlQuoteValue(D26,AllTriggers)</f>
-        <v>3.3571E-3</v>
+        <v>3.3356999999999996E-3</v>
       </c>
       <c r="H26" s="99">
         <f>_xll.qlOvernightIndexedSwapFairRate(B26,_xll.ohTrigger(C26,InterestRatesTrigger))</f>
-        <v>6.1645769044616243E-4</v>
+        <v>5.9178082191774304E-4</v>
       </c>
       <c r="I26" s="100">
         <f t="shared" si="1"/>
-        <v>2.7406423095538376E-3</v>
+        <v>2.7439191780822565E-3</v>
       </c>
       <c r="J26" s="108" t="b">
         <f>NOT(ISERROR(I26))</f>
@@ -4646,24 +4583,24 @@
       <c r="M26" s="109"/>
       <c r="N26" s="111">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="O26" s="111">
         <f t="shared" si="3"/>
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="P26" s="111">
         <f t="shared" si="7"/>
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="Q26" s="108"/>
       <c r="R26" s="122">
         <f t="shared" si="8"/>
-        <v>44044.333333333328</v>
+        <v>44408.333333333328</v>
       </c>
       <c r="S26" s="122">
         <f t="shared" si="9"/>
-        <v>181.5</v>
+        <v>182.5</v>
       </c>
       <c r="T26" s="122">
         <v>1</v>
@@ -4676,7 +4613,7 @@
       </c>
       <c r="B27" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E27,F27,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00371#0001</v>
+        <v>obj_003b4#0000</v>
       </c>
       <c r="C27" s="12" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B27,OisEngine)</f>
@@ -4688,11 +4625,11 @@
       </c>
       <c r="E27" s="53">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,"12M","mf")</f>
-        <v>42165</v>
+        <v>42167</v>
       </c>
       <c r="F27" s="54">
         <f>_xll.qlInterestRateIndexMaturity(A27,E27)</f>
-        <v>42531</v>
+        <v>42534</v>
       </c>
       <c r="G27" s="27" t="e">
         <f>_xll.qlQuoteValue(D27,AllTriggers)</f>
@@ -4700,7 +4637,7 @@
       </c>
       <c r="H27" s="15">
         <f>_xll.qlOvernightIndexedSwapFairRate(B27,_xll.ohTrigger(C27,InterestRatesTrigger))</f>
-        <v>6.6570269691259166E-4</v>
+        <v>6.4097754136601206E-4</v>
       </c>
       <c r="I27" s="16" t="e">
         <f t="shared" si="1"/>
@@ -4725,19 +4662,19 @@
       </c>
       <c r="O27" s="112">
         <f t="shared" si="3"/>
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="P27" s="112">
         <f t="shared" si="7"/>
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="R27" s="91">
         <f t="shared" si="8"/>
-        <v>311467</v>
+        <v>312076.33333333331</v>
       </c>
       <c r="S27" s="91">
         <f t="shared" si="9"/>
-        <v>548</v>
+        <v>548.5</v>
       </c>
       <c r="T27" s="91">
         <v>1</v>
@@ -4784,7 +4721,7 @@
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
       <c r="G30" s="58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30" s="58" t="b">
         <v>1</v>
@@ -4809,11 +4746,11 @@
       </c>
       <c r="V30" s="117">
         <f>Z9</f>
-        <v>4.6722025163461978E-10</v>
+        <v>-4.7916534998041182E-13</v>
       </c>
       <c r="W30" s="13">
         <f>Z18</f>
-        <v>1.7017064290611148E-9</v>
+        <v>9.9010787776119224E-9</v>
       </c>
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.2">
@@ -4822,19 +4759,19 @@
       </c>
       <c r="G31" s="37">
         <f>_xll.ohFilter(I2:I3,J2:J3)</f>
-        <v>3.374945009063749E-4</v>
+        <v>3.375041095903847E-4</v>
       </c>
       <c r="H31" s="38">
         <f>_xll.ohFilter(I6:I9,J6:J9)</f>
-        <v>7.0890014526361477E-4</v>
+        <v>7.3356164383544631E-4</v>
       </c>
       <c r="I31" s="38">
         <f>_xll.ohFilter(I15:I18,J15:J18)</f>
-        <v>1.2006387619912279E-3</v>
+        <v>1.2014616438356411E-3</v>
       </c>
       <c r="J31" s="39">
         <f>_xll.ohFilter(I25:I26,J25:J26)</f>
-        <v>2.7406423095538376E-3</v>
+        <v>2.7439191780822565E-3</v>
       </c>
       <c r="M31" s="58" t="s">
         <v>45</v>
@@ -4845,11 +4782,11 @@
       </c>
       <c r="O31" s="57">
         <f>K9</f>
-        <v>6.264397388355933E-10</v>
+        <v>1.3454955428348427E-7</v>
       </c>
       <c r="P31" s="57">
         <f>AVERAGE(K19:K21)</f>
-        <v>-3.331718970181937E-8</v>
+        <v>-1.5723874883343609E-7</v>
       </c>
       <c r="Q31" s="57" t="e">
         <f>K26</f>
@@ -4860,11 +4797,11 @@
       </c>
       <c r="V31" s="63">
         <f>Z10</f>
-        <v>-5.5278217853959341E-8</v>
+        <v>2.6915852507036314E-7</v>
       </c>
       <c r="W31" s="16">
         <f>Z19</f>
-        <v>-4.7033049852535764E-7</v>
+        <v>-2.6582666433212201E-6</v>
       </c>
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.2">
@@ -4873,19 +4810,19 @@
       </c>
       <c r="G32" s="37">
         <f>IF(G31&lt;H31,G31,H31)</f>
-        <v>3.374945009063749E-4</v>
+        <v>3.375041095903847E-4</v>
       </c>
       <c r="H32" s="38">
         <f>H31</f>
-        <v>7.0890014526361477E-4</v>
+        <v>7.3356164383544631E-4</v>
       </c>
       <c r="I32" s="38">
         <f>IF(I31&lt;H31,H31,I31)</f>
-        <v>1.2006387619912279E-3</v>
+        <v>1.2014616438356411E-3</v>
       </c>
       <c r="J32" s="39">
         <f>IF(J31&lt;I31,I31,J31)</f>
-        <v>2.7406423095538376E-3</v>
+        <v>2.7439191780822565E-3</v>
       </c>
       <c r="M32" s="58" t="s">
         <v>44</v>
@@ -4896,11 +4833,11 @@
       </c>
       <c r="O32" s="57">
         <f>L9</f>
-        <v>7.0884313924738068E-4</v>
+        <v>7.2118308484136573E-4</v>
       </c>
       <c r="P32" s="57">
         <f>L18</f>
-        <v>1.2066691733272571E-3</v>
+        <v>1.23023633487216E-3</v>
       </c>
       <c r="Q32" s="57" t="e">
         <f>L26</f>
@@ -4911,11 +4848,11 @@
       </c>
       <c r="V32" s="63">
         <f>Z11</f>
-        <v>7.1011129245365876E-4</v>
+        <v>7.2118170356738317E-4</v>
       </c>
       <c r="W32" s="16">
         <f>Z20</f>
-        <v>1.2245172338102538E-3</v>
+        <v>1.3341672993050476E-3</v>
       </c>
     </row>
     <row r="33" spans="2:23" x14ac:dyDescent="0.2">
@@ -4973,7 +4910,7 @@
     <row r="34" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B34" s="123" t="str">
         <f>_xll.qlMakeDatedOIS(,E34,F34,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_0035f#0001</v>
+        <v>obj_003a3#0000</v>
       </c>
       <c r="C34" s="7" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B34,OisEngine)</f>
@@ -4984,27 +4921,27 @@
       </c>
       <c r="E34" s="51">
         <f t="shared" ref="E34:E49" si="13">SettlementDate</f>
-        <v>41800</v>
+        <v>41802</v>
       </c>
       <c r="F34" s="22">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,D34,"Following")</f>
-        <v>41801</v>
-      </c>
-      <c r="G34" s="32" t="e">
+        <v>41803</v>
+      </c>
+      <c r="G34" s="32">
         <f t="shared" ref="G34:J38" si="14">$L34+IF(G$30,G$32,N34)</f>
-        <v>#NUM!</v>
+        <v>9.7225504479804342E-4</v>
       </c>
       <c r="H34" s="32">
         <f t="shared" si="14"/>
-        <v>1.350231326956116E-3</v>
+        <v>1.3683125790431051E-3</v>
       </c>
       <c r="I34" s="32">
         <f t="shared" si="14"/>
-        <v>1.841969943683729E-3</v>
+        <v>1.8362125790432997E-3</v>
       </c>
       <c r="J34" s="32">
         <f t="shared" si="14"/>
-        <v>3.3819734912463387E-3</v>
+        <v>3.3786701132899151E-3</v>
       </c>
       <c r="K34" s="124">
         <f>F34-$E$6</f>
@@ -5012,7 +4949,7 @@
       </c>
       <c r="L34" s="2">
         <f>L35</f>
-        <v>6.4133118169250119E-4</v>
+        <v>6.3475093520765872E-4</v>
       </c>
       <c r="N34" s="62" t="e">
         <f>N$31*$K34+N$32</f>
@@ -5020,11 +4957,11 @@
       </c>
       <c r="O34" s="63">
         <f t="shared" ref="O34:P40" si="15">IF(O$30,V34,O$31*$K34+O$32)</f>
-        <v>7.1008380908481566E-4</v>
+        <v>7.2131628267019655E-4</v>
       </c>
       <c r="P34" s="63">
         <f t="shared" si="15"/>
-        <v>1.2242826357964675E-3</v>
+        <v>1.3328414663429794E-3</v>
       </c>
       <c r="Q34" s="16" t="e">
         <f t="shared" ref="Q34:Q49" si="16">Q$31*$K34+Q$32</f>
@@ -5035,17 +4972,17 @@
       </c>
       <c r="V34" s="63">
         <f t="shared" ref="V34:W40" si="17">$K34*$K34/3*V$30+$K34/2*V$31+V$32</f>
-        <v>7.1008380908481566E-4</v>
+        <v>7.2131628267019655E-4</v>
       </c>
       <c r="W34" s="16">
         <f t="shared" si="17"/>
-        <v>1.2242826357964675E-3</v>
+        <v>1.3328414663429794E-3</v>
       </c>
     </row>
     <row r="35" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B35" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E35,F35,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00368#0001</v>
+        <v>obj_003a6#0000</v>
       </c>
       <c r="C35" s="5" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B35,OisEngine)</f>
@@ -5056,27 +4993,27 @@
       </c>
       <c r="E35" s="53">
         <f t="shared" si="13"/>
-        <v>41800</v>
+        <v>41802</v>
       </c>
       <c r="F35" s="24">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,D35,"Following")</f>
-        <v>41807</v>
-      </c>
-      <c r="G35" s="32" t="e">
+        <v>41809</v>
+      </c>
+      <c r="G35" s="32">
         <f t="shared" si="14"/>
-        <v>#NUM!</v>
+        <v>9.7225504479804342E-4</v>
       </c>
       <c r="H35" s="32">
         <f t="shared" si="14"/>
-        <v>1.350231326956116E-3</v>
+        <v>1.3683125790431051E-3</v>
       </c>
       <c r="I35" s="32">
         <f t="shared" si="14"/>
-        <v>1.841969943683729E-3</v>
+        <v>1.8362125790432997E-3</v>
       </c>
       <c r="J35" s="32">
         <f t="shared" si="14"/>
-        <v>3.3819734912463387E-3</v>
+        <v>3.3786701132899151E-3</v>
       </c>
       <c r="K35" s="125">
         <f t="shared" ref="K35:K49" si="18">F35-$E$6</f>
@@ -5084,7 +5021,7 @@
       </c>
       <c r="L35" s="3">
         <f>_xll.qlOvernightIndexedSwapFairRate(B35,_xll.ohTrigger(C35,InterestRatesTrigger))</f>
-        <v>6.4133118169250119E-4</v>
+        <v>6.3475093520765872E-4</v>
       </c>
       <c r="N35" s="62" t="e">
         <f>N$31*$K35+N$32</f>
@@ -5092,11 +5029,11 @@
       </c>
       <c r="O35" s="63">
         <f t="shared" si="15"/>
-        <v>7.0992544995527999E-4</v>
+        <v>7.2212375057876209E-4</v>
       </c>
       <c r="P35" s="63">
         <f t="shared" si="15"/>
-        <v>1.2228988716037564E-3</v>
+        <v>1.3250250836734576E-3</v>
       </c>
       <c r="Q35" s="16" t="e">
         <f t="shared" si="16"/>
@@ -5107,17 +5044,17 @@
       </c>
       <c r="V35" s="63">
         <f t="shared" si="17"/>
-        <v>7.0992544995527999E-4</v>
+        <v>7.2212375057876209E-4</v>
       </c>
       <c r="W35" s="16">
         <f t="shared" si="17"/>
-        <v>1.2228988716037564E-3</v>
+        <v>1.3250250836734576E-3</v>
       </c>
     </row>
     <row r="36" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B36" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E36,F36,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00364#0001</v>
+        <v>obj_003a8#0000</v>
       </c>
       <c r="C36" s="5" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B36,OisEngine)</f>
@@ -5128,27 +5065,27 @@
       </c>
       <c r="E36" s="53">
         <f t="shared" si="13"/>
-        <v>41800</v>
+        <v>41802</v>
       </c>
       <c r="F36" s="24">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,D36,"Following")</f>
-        <v>41814</v>
-      </c>
-      <c r="G36" s="32" t="e">
+        <v>41816</v>
+      </c>
+      <c r="G36" s="32">
         <f t="shared" si="14"/>
-        <v>#NUM!</v>
+        <v>9.7332253008677861E-4</v>
       </c>
       <c r="H36" s="32">
         <f t="shared" si="14"/>
-        <v>1.3501844066998643E-3</v>
+        <v>1.3693800643318401E-3</v>
       </c>
       <c r="I36" s="32">
         <f t="shared" si="14"/>
-        <v>1.8419230234274775E-3</v>
+        <v>1.8372800643320351E-3</v>
       </c>
       <c r="J36" s="32">
         <f t="shared" si="14"/>
-        <v>3.3819265709900872E-3</v>
+        <v>3.3797375985786505E-3</v>
       </c>
       <c r="K36" s="125">
         <f t="shared" si="18"/>
@@ -5156,7 +5093,7 @@
       </c>
       <c r="L36" s="3">
         <f>_xll.qlOvernightIndexedSwapFairRate(B36,_xll.ohTrigger(C36,InterestRatesTrigger))</f>
-        <v>6.412842614362496E-4</v>
+        <v>6.3581842049639391E-4</v>
       </c>
       <c r="N36" s="62" t="e">
         <f>N$31*$K36+N$32</f>
@@ -5164,11 +5101,11 @@
       </c>
       <c r="O36" s="63">
         <f t="shared" si="15"/>
-        <v>7.0975486998512121E-4</v>
+        <v>7.2306578193740616E-4</v>
       </c>
       <c r="P36" s="63">
         <f t="shared" si="15"/>
-        <v>1.2213360984739416E-3</v>
+        <v>1.3162063032819363E-3</v>
       </c>
       <c r="Q36" s="16" t="e">
         <f t="shared" si="16"/>
@@ -5179,17 +5116,17 @@
       </c>
       <c r="V36" s="63">
         <f t="shared" si="17"/>
-        <v>7.0975486998512121E-4</v>
+        <v>7.2306578193740616E-4</v>
       </c>
       <c r="W36" s="16">
         <f t="shared" si="17"/>
-        <v>1.2213360984739416E-3</v>
+        <v>1.3162063032819363E-3</v>
       </c>
     </row>
     <row r="37" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B37" s="30" t="str">
         <f>_xll.qlMakeDatedOIS(,E37,F37,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_0036a#0001</v>
+        <v>obj_003aa#0000</v>
       </c>
       <c r="C37" s="10" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B37,OisEngine)</f>
@@ -5200,27 +5137,27 @@
       </c>
       <c r="E37" s="52">
         <f t="shared" si="13"/>
-        <v>41800</v>
+        <v>41802</v>
       </c>
       <c r="F37" s="26">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,D37,"Following")</f>
-        <v>41821</v>
-      </c>
-      <c r="G37" s="35" t="e">
+        <v>41823</v>
+      </c>
+      <c r="G37" s="35">
         <f t="shared" si="14"/>
-        <v>#NUM!</v>
+        <v>9.7494152837839963E-4</v>
       </c>
       <c r="H37" s="35">
         <f>$L37+IF(H$30,H$32,O37)</f>
-        <v>1.3501158829284452E-3</v>
+        <v>1.3709990626234612E-3</v>
       </c>
       <c r="I37" s="35">
         <f t="shared" si="14"/>
-        <v>1.8418544996560583E-3</v>
+        <v>1.838899062623656E-3</v>
       </c>
       <c r="J37" s="35">
         <f t="shared" si="14"/>
-        <v>3.381858047218668E-3</v>
+        <v>3.3813565968702714E-3</v>
       </c>
       <c r="K37" s="126">
         <f t="shared" si="18"/>
@@ -5228,7 +5165,7 @@
       </c>
       <c r="L37" s="4">
         <f>_xll.qlOvernightIndexedSwapFairRate(B37,_xll.ohTrigger(C37,InterestRatesTrigger))</f>
-        <v>6.4121573766483047E-4</v>
+        <v>6.3743741878801493E-4</v>
       </c>
       <c r="N37" s="92" t="e">
         <f>N$31*$K37+N$32</f>
@@ -5236,11 +5173,11 @@
       </c>
       <c r="O37" s="93">
         <f t="shared" si="15"/>
-        <v>7.0959955254318243E-4</v>
+        <v>7.2400779764331558E-4</v>
       </c>
       <c r="P37" s="93">
         <f t="shared" si="15"/>
-        <v>1.2198289144208095E-3</v>
+        <v>1.3077109581304837E-3</v>
       </c>
       <c r="Q37" s="14" t="e">
         <f t="shared" si="16"/>
@@ -5251,17 +5188,17 @@
       </c>
       <c r="V37" s="93">
         <f t="shared" si="17"/>
-        <v>7.0959955254318243E-4</v>
+        <v>7.2400779764331558E-4</v>
       </c>
       <c r="W37" s="14">
         <f t="shared" si="17"/>
-        <v>1.2198289144208095E-3</v>
+        <v>1.3077109581304837E-3</v>
       </c>
     </row>
     <row r="38" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B38" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E38,F38,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00369#0001</v>
+        <v>obj_003a7#0000</v>
       </c>
       <c r="C38" s="5" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B38,OisEngine)</f>
@@ -5272,35 +5209,35 @@
       </c>
       <c r="E38" s="53">
         <f t="shared" si="13"/>
-        <v>41800</v>
+        <v>41802</v>
       </c>
       <c r="F38" s="24">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,D38,"mf",TRUE)</f>
-        <v>41830</v>
-      </c>
-      <c r="G38" s="34" t="e">
+        <v>41834</v>
+      </c>
+      <c r="G38" s="34">
         <f t="shared" si="14"/>
-        <v>#NUM!</v>
+        <v>9.7860000000000004E-4</v>
       </c>
       <c r="H38" s="34">
         <f t="shared" si="14"/>
-        <v>1.3499960356755617E-3</v>
+        <v>1.3746575342450617E-3</v>
       </c>
       <c r="I38" s="34">
         <f t="shared" si="14"/>
-        <v>1.8417346524031747E-3</v>
+        <v>1.8425575342452564E-3</v>
       </c>
       <c r="J38" s="34">
         <f t="shared" si="14"/>
-        <v>3.3817381999657844E-3</v>
+        <v>3.3850150684918718E-3</v>
       </c>
       <c r="K38" s="124">
         <f t="shared" si="18"/>
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L38" s="3">
         <f>_xll.qlOvernightIndexedSwapFairRate(B38,_xll.ohTrigger(C38,InterestRatesTrigger))</f>
-        <v>6.4109589041194692E-4</v>
+        <v>6.4109589040961534E-4</v>
       </c>
       <c r="N38" s="62" t="e">
         <f>N$31*$K38+N$32</f>
@@ -5308,11 +5245,11 @@
       </c>
       <c r="O38" s="63">
         <f t="shared" si="15"/>
-        <v>7.0942228526133975E-4</v>
+        <v>7.2548807641340288E-4</v>
       </c>
       <c r="P38" s="63">
         <f t="shared" si="15"/>
-        <v>1.2179727882610917E-3</v>
+        <v>1.2950146012346664E-3</v>
       </c>
       <c r="Q38" s="16" t="e">
         <f t="shared" si="16"/>
@@ -5323,17 +5260,17 @@
       </c>
       <c r="V38" s="63">
         <f t="shared" si="17"/>
-        <v>7.0942228526133975E-4</v>
+        <v>7.2548807641340288E-4</v>
       </c>
       <c r="W38" s="16">
         <f t="shared" si="17"/>
-        <v>1.2179727882610917E-3</v>
+        <v>1.2950146012346664E-3</v>
       </c>
     </row>
     <row r="39" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B39" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E39,F39,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00362#0001</v>
+        <v>obj_003ac#0000</v>
       </c>
       <c r="C39" s="5" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B39,OisEngine)</f>
@@ -5344,41 +5281,41 @@
       </c>
       <c r="E39" s="53">
         <f t="shared" si="13"/>
-        <v>41800</v>
+        <v>41802</v>
       </c>
       <c r="F39" s="24">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,D39,"mf",TRUE)</f>
-        <v>41862</v>
+        <v>41863</v>
       </c>
       <c r="G39" s="47"/>
       <c r="H39" s="32">
         <f t="shared" ref="H39:J40" si="19">$L39+IF(H$30,H$32,O39)</f>
-        <v>1.3499960356743582E-3</v>
+        <v>1.3746575342467816E-3</v>
       </c>
       <c r="I39" s="32">
         <f t="shared" si="19"/>
-        <v>1.8417346524019712E-3</v>
+        <v>1.8425575342469764E-3</v>
       </c>
       <c r="J39" s="32">
         <f t="shared" si="19"/>
-        <v>3.3817381999645809E-3</v>
+        <v>3.3850150684935918E-3</v>
       </c>
       <c r="K39" s="125">
         <f t="shared" si="18"/>
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L39" s="3">
         <f>_xll.qlOvernightIndexedSwapFairRate(B39,_xll.ohTrigger(C39,InterestRatesTrigger))</f>
-        <v>6.4109589041074346E-4</v>
+        <v>6.4109589041133532E-4</v>
       </c>
       <c r="N39" s="47"/>
       <c r="O39" s="63">
         <f t="shared" si="15"/>
-        <v>7.0899633258261383E-4</v>
+        <v>7.2939044425727345E-4</v>
       </c>
       <c r="P39" s="63">
         <f t="shared" si="15"/>
-        <v>1.2121174415270714E-3</v>
+        <v>1.2653708047275817E-3</v>
       </c>
       <c r="Q39" s="16" t="e">
         <f t="shared" si="16"/>
@@ -5389,17 +5326,17 @@
       </c>
       <c r="V39" s="63">
         <f t="shared" si="17"/>
-        <v>7.0899633258261383E-4</v>
+        <v>7.2939044425727345E-4</v>
       </c>
       <c r="W39" s="16">
         <f t="shared" si="17"/>
-        <v>1.2121174415270714E-3</v>
+        <v>1.2653708047275817E-3</v>
       </c>
     </row>
     <row r="40" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B40" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E40,F40,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00363#0001</v>
+        <v>obj_003ad#0000</v>
       </c>
       <c r="C40" s="5" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B40,OisEngine)</f>
@@ -5410,24 +5347,24 @@
       </c>
       <c r="E40" s="53">
         <f t="shared" si="13"/>
-        <v>41800</v>
+        <v>41802</v>
       </c>
       <c r="F40" s="24">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,D40,"mf",TRUE)</f>
-        <v>41892</v>
+        <v>41894</v>
       </c>
       <c r="G40" s="45"/>
       <c r="H40" s="32">
         <f t="shared" si="19"/>
-        <v>1.3499960356747507E-3</v>
+        <v>1.3500000000000001E-3</v>
       </c>
       <c r="I40" s="32">
         <f t="shared" si="19"/>
-        <v>1.8417346524023637E-3</v>
+        <v>1.8179000000001948E-3</v>
       </c>
       <c r="J40" s="32">
         <f t="shared" si="19"/>
-        <v>3.3817381999649734E-3</v>
+        <v>3.3603575342468104E-3</v>
       </c>
       <c r="K40" s="125">
         <f t="shared" si="18"/>
@@ -5435,16 +5372,16 @@
       </c>
       <c r="L40" s="3">
         <f>_xll.qlOvernightIndexedSwapFairRate(B40,_xll.ohTrigger(C40,InterestRatesTrigger))</f>
-        <v>6.4109589041113594E-4</v>
+        <v>6.1643835616455376E-4</v>
       </c>
       <c r="N40" s="45"/>
       <c r="O40" s="63">
         <f t="shared" si="15"/>
-        <v>7.0888667850232175E-4</v>
+        <v>7.3356164383544576E-4</v>
       </c>
       <c r="P40" s="63">
         <f t="shared" si="15"/>
-        <v>1.2076831119499452E-3</v>
+        <v>1.2398212773035073E-3</v>
       </c>
       <c r="Q40" s="16" t="e">
         <f t="shared" si="16"/>
@@ -5455,17 +5392,17 @@
       </c>
       <c r="V40" s="63">
         <f t="shared" si="17"/>
-        <v>7.0888667850232175E-4</v>
+        <v>7.3356164383544576E-4</v>
       </c>
       <c r="W40" s="16">
         <f t="shared" si="17"/>
-        <v>1.2076831119499452E-3</v>
+        <v>1.2398212773035073E-3</v>
       </c>
     </row>
     <row r="41" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B41" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E41,F41,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_0036b#0001</v>
+        <v>obj_003a0#0000</v>
       </c>
       <c r="C41" s="5" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B41,OisEngine)</f>
@@ -5476,35 +5413,35 @@
       </c>
       <c r="E41" s="53">
         <f t="shared" si="13"/>
-        <v>41800</v>
+        <v>41802</v>
       </c>
       <c r="F41" s="24">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,D41,"mf",TRUE)</f>
-        <v>41922</v>
+        <v>41926</v>
       </c>
       <c r="G41" s="36"/>
       <c r="H41" s="46"/>
       <c r="I41" s="32">
         <f t="shared" ref="I41:J43" si="20">$L41+IF(I$30,I$32,P41)</f>
-        <v>1.8417346524025632E-3</v>
+        <v>1.8179000000003629E-3</v>
       </c>
       <c r="J41" s="32">
         <f t="shared" si="20"/>
-        <v>3.3817381999651729E-3</v>
+        <v>3.3603575342469783E-3</v>
       </c>
       <c r="K41" s="125">
         <f t="shared" si="18"/>
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="L41" s="3">
         <f>_xll.qlOvernightIndexedSwapFairRate(B41,_xll.ohTrigger(C41,InterestRatesTrigger))</f>
-        <v>6.4109589041133521E-4</v>
+        <v>6.1643835616472192E-4</v>
       </c>
       <c r="N41" s="36"/>
       <c r="O41" s="46"/>
       <c r="P41" s="63">
         <f>IF(P$30,W41,P$31*$K41+P$32)</f>
-        <v>1.2042698062302555E-3</v>
+        <v>1.2201010965139855E-3</v>
       </c>
       <c r="Q41" s="16" t="e">
         <f t="shared" si="16"/>
@@ -5516,13 +5453,13 @@
       <c r="V41" s="63"/>
       <c r="W41" s="16">
         <f>$K41*$K41/3*W$30+$K41/2*W$31+W$32</f>
-        <v>1.2042698062302555E-3</v>
+        <v>1.2201010965139855E-3</v>
       </c>
     </row>
     <row r="42" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B42" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E42,F42,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00367#0001</v>
+        <v>obj_003a4#0000</v>
       </c>
       <c r="C42" s="5" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B42,OisEngine)</f>
@@ -5533,21 +5470,21 @@
       </c>
       <c r="E42" s="53">
         <f t="shared" si="13"/>
-        <v>41800</v>
+        <v>41802</v>
       </c>
       <c r="F42" s="24">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,D42,"mf",TRUE)</f>
-        <v>41953</v>
+        <v>41955</v>
       </c>
       <c r="G42" s="36"/>
       <c r="H42" s="44"/>
       <c r="I42" s="32">
         <f t="shared" si="20"/>
-        <v>1.8417346524024435E-3</v>
+        <v>1.8179000000002913E-3</v>
       </c>
       <c r="J42" s="32">
         <f t="shared" si="20"/>
-        <v>3.3817381999650532E-3</v>
+        <v>3.3603575342469067E-3</v>
       </c>
       <c r="K42" s="125">
         <f t="shared" si="18"/>
@@ -5555,13 +5492,13 @@
       </c>
       <c r="L42" s="3">
         <f>_xll.qlOvernightIndexedSwapFairRate(B42,_xll.ohTrigger(C42,InterestRatesTrigger))</f>
-        <v>6.4109589041121552E-4</v>
+        <v>6.1643835616465015E-4</v>
       </c>
       <c r="N42" s="36"/>
       <c r="O42" s="44"/>
       <c r="P42" s="63">
         <f>IF(P$30,W42,P$31*$K42+P$32)</f>
-        <v>1.2018153659390277E-3</v>
+        <v>1.2080680187926802E-3</v>
       </c>
       <c r="Q42" s="16" t="e">
         <f t="shared" si="16"/>
@@ -5573,13 +5510,13 @@
       <c r="V42" s="63"/>
       <c r="W42" s="16">
         <f>$K42*$K42/3*W$30+$K42/2*W$31+W$32</f>
-        <v>1.2018153659390277E-3</v>
+        <v>1.2080680187926802E-3</v>
       </c>
     </row>
     <row r="43" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B43" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E43,F43,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00360#0001</v>
+        <v>obj_003a5#0000</v>
       </c>
       <c r="C43" s="5" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B43,OisEngine)</f>
@@ -5590,21 +5527,21 @@
       </c>
       <c r="E43" s="53">
         <f t="shared" si="13"/>
-        <v>41800</v>
+        <v>41802</v>
       </c>
       <c r="F43" s="24">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,D43,"mf",TRUE)</f>
-        <v>41983</v>
+        <v>41985</v>
       </c>
       <c r="G43" s="36"/>
       <c r="H43" s="44"/>
       <c r="I43" s="32">
         <f t="shared" si="20"/>
-        <v>1.8170771181555872E-3</v>
+        <v>1.8179000000000003E-3</v>
       </c>
       <c r="J43" s="32">
         <f t="shared" si="20"/>
-        <v>3.3570806657181968E-3</v>
+        <v>3.3603575342466157E-3</v>
       </c>
       <c r="K43" s="125">
         <f t="shared" si="18"/>
@@ -5618,7 +5555,7 @@
       <c r="O43" s="44"/>
       <c r="P43" s="63">
         <f>IF(P$30,W43,P$31*$K43+P$32)</f>
-        <v>1.2004781420627928E-3</v>
+        <v>1.2014616438356378E-3</v>
       </c>
       <c r="Q43" s="16" t="e">
         <f t="shared" si="16"/>
@@ -5630,13 +5567,13 @@
       <c r="V43" s="93"/>
       <c r="W43" s="14">
         <f>$K43*$K43/3*W$30+$K43/2*W$31+W$32</f>
-        <v>1.2004781420627928E-3</v>
+        <v>1.2014616438356378E-3</v>
       </c>
     </row>
     <row r="44" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B44" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E44,F44,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_0035c#0001</v>
+        <v>obj_003a9#0000</v>
       </c>
       <c r="C44" s="5" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B44,OisEngine)</f>
@@ -5647,7 +5584,7 @@
       </c>
       <c r="E44" s="53">
         <f t="shared" si="13"/>
-        <v>41800</v>
+        <v>41802</v>
       </c>
       <c r="F44" s="24">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,D44,"mf",TRUE)</f>
@@ -5658,15 +5595,15 @@
       <c r="I44" s="46"/>
       <c r="J44" s="32">
         <f t="shared" ref="J44:J49" si="21">$L44+IF(J$30,J$32,Q44)</f>
-        <v>3.3486393057430238E-3</v>
+        <v>3.3629798388215282E-3</v>
       </c>
       <c r="K44" s="125">
         <f t="shared" si="18"/>
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="L44" s="3">
         <f>_xll.qlOvernightIndexedSwapFairRate(B44,_xll.ohTrigger(C44,InterestRatesTrigger))</f>
-        <v>6.0799699618918623E-4</v>
+        <v>6.1906066073927151E-4</v>
       </c>
       <c r="N44" s="36"/>
       <c r="O44" s="33"/>
@@ -5679,7 +5616,7 @@
     <row r="45" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B45" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E45,F45,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_0035d#0001</v>
+        <v>obj_0039f#0000</v>
       </c>
       <c r="C45" s="5" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B45,OisEngine)</f>
@@ -5690,18 +5627,18 @@
       </c>
       <c r="E45" s="53">
         <f t="shared" si="13"/>
-        <v>41800</v>
+        <v>41802</v>
       </c>
       <c r="F45" s="24">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,D45,"mf",TRUE)</f>
-        <v>42045</v>
+        <v>42047</v>
       </c>
       <c r="G45" s="36"/>
       <c r="H45" s="33"/>
       <c r="I45" s="44"/>
       <c r="J45" s="32">
         <f t="shared" si="21"/>
-        <v>3.3526315869634102E-3</v>
+        <v>3.3638434898536572E-3</v>
       </c>
       <c r="K45" s="125">
         <f t="shared" si="18"/>
@@ -5709,7 +5646,7 @@
       </c>
       <c r="L45" s="3">
         <f>_xll.qlOvernightIndexedSwapFairRate(B45,_xll.ohTrigger(C45,InterestRatesTrigger))</f>
-        <v>6.1198927740957238E-4</v>
+        <v>6.199243117714009E-4</v>
       </c>
       <c r="N45" s="36"/>
       <c r="O45" s="33"/>
@@ -5722,7 +5659,7 @@
     <row r="46" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B46" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E46,F46,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00365#0001</v>
+        <v>obj_003ae#0000</v>
       </c>
       <c r="C46" s="5" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B46,OisEngine)</f>
@@ -5733,18 +5670,18 @@
       </c>
       <c r="E46" s="53">
         <f t="shared" si="13"/>
-        <v>41800</v>
+        <v>41802</v>
       </c>
       <c r="F46" s="24">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,D46,"mf",TRUE)</f>
-        <v>42073</v>
+        <v>42075</v>
       </c>
       <c r="G46" s="36"/>
       <c r="H46" s="33"/>
       <c r="I46" s="44"/>
       <c r="J46" s="32">
         <f t="shared" si="21"/>
-        <v>3.357080665718E-3</v>
+        <v>3.3603575342467116E-3</v>
       </c>
       <c r="K46" s="125">
         <f t="shared" si="18"/>
@@ -5752,7 +5689,7 @@
       </c>
       <c r="L46" s="3">
         <f>_xll.qlOvernightIndexedSwapFairRate(B46,_xll.ohTrigger(C46,InterestRatesTrigger))</f>
-        <v>6.1643835616416226E-4</v>
+        <v>6.164383561644551E-4</v>
       </c>
       <c r="N46" s="36"/>
       <c r="O46" s="33"/>
@@ -5765,7 +5702,7 @@
     <row r="47" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B47" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E47,F47,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00366#0001</v>
+        <v>obj_003a1#0000</v>
       </c>
       <c r="C47" s="5" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B47,OisEngine)</f>
@@ -5776,26 +5713,26 @@
       </c>
       <c r="E47" s="53">
         <f t="shared" si="13"/>
-        <v>41800</v>
+        <v>41802</v>
       </c>
       <c r="F47" s="24">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,D47,"mf",TRUE)</f>
-        <v>42104</v>
+        <v>42107</v>
       </c>
       <c r="G47" s="36"/>
       <c r="H47" s="33"/>
       <c r="I47" s="44"/>
       <c r="J47" s="32">
         <f t="shared" si="21"/>
-        <v>3.3578338171418496E-3</v>
+        <v>3.3508758742490548E-3</v>
       </c>
       <c r="K47" s="125">
         <f t="shared" si="18"/>
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="L47" s="3">
         <f>_xll.qlOvernightIndexedSwapFairRate(B47,_xll.ohTrigger(C47,InterestRatesTrigger))</f>
-        <v>6.1719150758801199E-4</v>
+        <v>6.0695669616679822E-4</v>
       </c>
       <c r="N47" s="36"/>
       <c r="O47" s="33"/>
@@ -5808,7 +5745,7 @@
     <row r="48" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B48" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E48,F48,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00361#0001</v>
+        <v>obj_003ab#0000</v>
       </c>
       <c r="C48" s="5" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B48,OisEngine)</f>
@@ -5819,26 +5756,26 @@
       </c>
       <c r="E48" s="53">
         <f t="shared" si="13"/>
-        <v>41800</v>
+        <v>41802</v>
       </c>
       <c r="F48" s="24">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,D48,"mf",TRUE)</f>
-        <v>42135</v>
+        <v>42136</v>
       </c>
       <c r="G48" s="36"/>
       <c r="H48" s="33"/>
       <c r="I48" s="44"/>
       <c r="J48" s="32">
         <f t="shared" si="21"/>
-        <v>3.3568298895549249E-3</v>
+        <v>3.3417270652012013E-3</v>
       </c>
       <c r="K48" s="125">
         <f t="shared" si="18"/>
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="L48" s="3">
         <f>_xll.qlOvernightIndexedSwapFairRate(B48,_xll.ohTrigger(C48,InterestRatesTrigger))</f>
-        <v>6.1618758000108723E-4</v>
+        <v>5.9780788711894493E-4</v>
       </c>
       <c r="N48" s="36"/>
       <c r="O48" s="33"/>
@@ -5851,7 +5788,7 @@
     <row r="49" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B49" s="30" t="str">
         <f>_xll.qlMakeDatedOIS(,E49,F49,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_0035e#0001</v>
+        <v>obj_003a2#0000</v>
       </c>
       <c r="C49" s="10" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B49,OisEngine)</f>
@@ -5862,18 +5799,18 @@
       </c>
       <c r="E49" s="53">
         <f t="shared" si="13"/>
-        <v>41800</v>
+        <v>41802</v>
       </c>
       <c r="F49" s="24">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,D49,"mf",TRUE)</f>
-        <v>42165</v>
+        <v>42167</v>
       </c>
       <c r="G49" s="36"/>
       <c r="H49" s="33"/>
       <c r="I49" s="44"/>
       <c r="J49" s="32">
         <f t="shared" si="21"/>
-        <v>3.3570806657183174E-3</v>
+        <v>3.3356999999999996E-3</v>
       </c>
       <c r="K49" s="125">
         <f t="shared" si="18"/>
@@ -5881,7 +5818,7 @@
       </c>
       <c r="L49" s="3">
         <f>_xll.qlOvernightIndexedSwapFairRate(B49,_xll.ohTrigger(C49,InterestRatesTrigger))</f>
-        <v>6.1643835616447993E-4</v>
+        <v>5.9178082191774304E-4</v>
       </c>
       <c r="N49" s="64"/>
       <c r="O49" s="65"/>
@@ -5920,7 +5857,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5990,7 +5927,7 @@
       </c>
       <c r="P2" s="215">
         <f>_xll.ohTrigger(O3:O7)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
@@ -6017,22 +5954,22 @@
       <c r="I3" s="163" t="s">
         <v>54</v>
       </c>
-      <c r="J3" s="218" t="e">
+      <c r="J3" s="218">
         <f>ROUND(Depo_Calculation!$G34,6)</f>
-        <v>#NUM!</v>
+        <v>9.7199999999999999E-4</v>
       </c>
       <c r="K3" s="156"/>
       <c r="L3" s="166">
         <v>1.488E-3</v>
       </c>
       <c r="M3" s="140"/>
-      <c r="N3" s="169" t="e">
+      <c r="N3" s="169">
         <f t="array" ref="N3:N40">QuoteLive</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="O3" s="170" t="e">
+        <v>9.7199999999999999E-4</v>
+      </c>
+      <c r="O3" s="170">
         <f>_xll.qlSimpleQuoteSetValue(D3,ROUND(N3,6),EvaluationDate)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="P3" s="190"/>
     </row>
@@ -6061,21 +5998,21 @@
       <c r="I4" s="163" t="s">
         <v>55</v>
       </c>
-      <c r="J4" s="218" t="e">
+      <c r="J4" s="218">
         <f>ROUND(Depo_Calculation!$G35,6)</f>
-        <v>#NUM!</v>
+        <v>9.7199999999999999E-4</v>
       </c>
       <c r="K4" s="156"/>
       <c r="L4" s="166">
         <v>1.4840000000000001E-3</v>
       </c>
       <c r="M4" s="140"/>
-      <c r="N4" s="169" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="O4" s="170" t="e">
+      <c r="N4" s="169">
+        <v>9.7199999999999999E-4</v>
+      </c>
+      <c r="O4" s="170">
         <f>_xll.qlSimpleQuoteSetValue(D4,ROUND(N4,6),EvaluationDate)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="P4" s="190"/>
     </row>
@@ -6101,21 +6038,21 @@
       <c r="I5" s="163" t="s">
         <v>56</v>
       </c>
-      <c r="J5" s="218" t="e">
+      <c r="J5" s="218">
         <f>ROUND(Depo_Calculation!$G36,6)</f>
-        <v>#NUM!</v>
+        <v>9.7300000000000002E-4</v>
       </c>
       <c r="K5" s="156"/>
       <c r="L5" s="166">
         <v>1.5E-3</v>
       </c>
       <c r="M5" s="140"/>
-      <c r="N5" s="169" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="O5" s="170" t="e">
+      <c r="N5" s="169">
+        <v>9.7300000000000002E-4</v>
+      </c>
+      <c r="O5" s="170">
         <f>_xll.qlSimpleQuoteSetValue(D5,ROUND(N5,6),EvaluationDate)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="P5" s="190"/>
     </row>
@@ -6141,21 +6078,21 @@
       <c r="I6" s="164" t="s">
         <v>57</v>
       </c>
-      <c r="J6" s="220" t="e">
+      <c r="J6" s="220">
         <f>Depo_Calculation!$G37</f>
-        <v>#NUM!</v>
+        <v>9.7494152837839963E-4</v>
       </c>
       <c r="K6" s="156"/>
       <c r="L6" s="167">
         <v>1.5054706107835709E-3</v>
       </c>
       <c r="M6" s="140"/>
-      <c r="N6" s="171" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="O6" s="170" t="e">
+      <c r="N6" s="171">
+        <v>9.7494152837839963E-4</v>
+      </c>
+      <c r="O6" s="170">
         <f>_xll.qlSimpleQuoteSetValue(D6,ROUND(N6,6),EvaluationDate)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="P6" s="190"/>
     </row>
@@ -6181,21 +6118,21 @@
       <c r="I7" s="165" t="s">
         <v>58</v>
       </c>
-      <c r="J7" s="219" t="e">
+      <c r="J7" s="219">
         <f>ROUND(Depo_Calculation!$G38,6)</f>
-        <v>#NUM!</v>
+        <v>9.7900000000000005E-4</v>
       </c>
       <c r="K7" s="156"/>
       <c r="L7" s="168">
         <v>1.5100000000000001E-3</v>
       </c>
       <c r="M7" s="140"/>
-      <c r="N7" s="172" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="O7" s="240" t="e">
+      <c r="N7" s="172">
+        <v>9.7900000000000005E-4</v>
+      </c>
+      <c r="O7" s="240">
         <f>_xll.qlSimpleQuoteSetValue(D7,ROUND(N7,6),EvaluationDate)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="P7" s="190"/>
     </row>
@@ -6225,7 +6162,7 @@
       </c>
       <c r="J8" s="217">
         <f>ROUND(Depo_Calculation!$H34,6)</f>
-        <v>1.3500000000000001E-3</v>
+        <v>1.3680000000000001E-3</v>
       </c>
       <c r="K8" s="156"/>
       <c r="L8" s="166">
@@ -6233,7 +6170,7 @@
       </c>
       <c r="M8" s="140"/>
       <c r="N8" s="169">
-        <v>1.3500000000000001E-3</v>
+        <v>1.3680000000000001E-3</v>
       </c>
       <c r="O8" s="239">
         <f>_xll.qlSimpleQuoteSetValue(D8,ROUND(N8,6),EvaluationDate)</f>
@@ -6241,7 +6178,7 @@
       </c>
       <c r="P8" s="216">
         <f>_xll.ohTrigger(O8:O14)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
@@ -6271,7 +6208,7 @@
       </c>
       <c r="J9" s="218">
         <f>ROUND(Depo_Calculation!$H35,6)</f>
-        <v>1.3500000000000001E-3</v>
+        <v>1.3680000000000001E-3</v>
       </c>
       <c r="K9" s="156"/>
       <c r="L9" s="166">
@@ -6279,7 +6216,7 @@
       </c>
       <c r="M9" s="140"/>
       <c r="N9" s="169">
-        <v>1.3500000000000001E-3</v>
+        <v>1.3680000000000001E-3</v>
       </c>
       <c r="O9" s="170">
         <f>_xll.qlSimpleQuoteSetValue(D9,ROUND(N9,6),EvaluationDate)</f>
@@ -6311,7 +6248,7 @@
       </c>
       <c r="J10" s="218">
         <f>ROUND(Depo_Calculation!$H36,6)</f>
-        <v>1.3500000000000001E-3</v>
+        <v>1.369E-3</v>
       </c>
       <c r="K10" s="156"/>
       <c r="L10" s="166">
@@ -6319,7 +6256,7 @@
       </c>
       <c r="M10" s="140"/>
       <c r="N10" s="169">
-        <v>1.3500000000000001E-3</v>
+        <v>1.369E-3</v>
       </c>
       <c r="O10" s="170">
         <f>_xll.qlSimpleQuoteSetValue(D10,ROUND(N10,6),EvaluationDate)</f>
@@ -6351,7 +6288,7 @@
       </c>
       <c r="J11" s="218">
         <f>ROUND(Depo_Calculation!$H37,6)</f>
-        <v>1.3500000000000001E-3</v>
+        <v>1.371E-3</v>
       </c>
       <c r="K11" s="156"/>
       <c r="L11" s="166">
@@ -6359,7 +6296,7 @@
       </c>
       <c r="M11" s="140"/>
       <c r="N11" s="169">
-        <v>1.3500000000000001E-3</v>
+        <v>1.371E-3</v>
       </c>
       <c r="O11" s="170">
         <f>_xll.qlSimpleQuoteSetValue(D11,ROUND(N11,6),EvaluationDate)</f>
@@ -6391,7 +6328,7 @@
       </c>
       <c r="J12" s="218">
         <f>ROUND(Depo_Calculation!$H38,6)</f>
-        <v>1.3500000000000001E-3</v>
+        <v>1.3749999999999999E-3</v>
       </c>
       <c r="K12" s="156"/>
       <c r="L12" s="166">
@@ -6399,7 +6336,7 @@
       </c>
       <c r="M12" s="140"/>
       <c r="N12" s="169">
-        <v>1.3500000000000001E-3</v>
+        <v>1.3749999999999999E-3</v>
       </c>
       <c r="O12" s="170">
         <f>_xll.qlSimpleQuoteSetValue(D12,ROUND(N12,6),EvaluationDate)</f>
@@ -6431,7 +6368,7 @@
       </c>
       <c r="J13" s="218">
         <f>ROUND(Depo_Calculation!$H39,6)</f>
-        <v>1.3500000000000001E-3</v>
+        <v>1.3749999999999999E-3</v>
       </c>
       <c r="K13" s="156"/>
       <c r="L13" s="166">
@@ -6439,7 +6376,7 @@
       </c>
       <c r="M13" s="140"/>
       <c r="N13" s="169">
-        <v>1.3500000000000001E-3</v>
+        <v>1.3749999999999999E-3</v>
       </c>
       <c r="O13" s="170">
         <f>_xll.qlSimpleQuoteSetValue(D13,ROUND(N13,6),EvaluationDate)</f>
@@ -6513,7 +6450,7 @@
       </c>
       <c r="J15" s="217">
         <f>ROUND(Depo_Calculation!$I34,6)</f>
-        <v>1.8420000000000001E-3</v>
+        <v>1.836E-3</v>
       </c>
       <c r="K15" s="156"/>
       <c r="L15" s="166">
@@ -6521,7 +6458,7 @@
       </c>
       <c r="M15" s="140"/>
       <c r="N15" s="169">
-        <v>1.8420000000000001E-3</v>
+        <v>1.836E-3</v>
       </c>
       <c r="O15" s="170">
         <f>_xll.qlSimpleQuoteSetValue(D15,ROUND(N15,6),EvaluationDate)</f>
@@ -6529,7 +6466,7 @@
       </c>
       <c r="P15" s="190">
         <f>_xll.ohTrigger(O15:O24)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
@@ -6559,7 +6496,7 @@
       </c>
       <c r="J16" s="218">
         <f>ROUND(Depo_Calculation!$I35,6)</f>
-        <v>1.8420000000000001E-3</v>
+        <v>1.836E-3</v>
       </c>
       <c r="K16" s="156"/>
       <c r="L16" s="166">
@@ -6567,7 +6504,7 @@
       </c>
       <c r="M16" s="140"/>
       <c r="N16" s="169">
-        <v>1.8420000000000001E-3</v>
+        <v>1.836E-3</v>
       </c>
       <c r="O16" s="170">
         <f>_xll.qlSimpleQuoteSetValue(D16,ROUND(N16,6),EvaluationDate)</f>
@@ -6599,7 +6536,7 @@
       </c>
       <c r="J17" s="218">
         <f>ROUND(Depo_Calculation!$I36,6)</f>
-        <v>1.8420000000000001E-3</v>
+        <v>1.8370000000000001E-3</v>
       </c>
       <c r="K17" s="156"/>
       <c r="L17" s="166">
@@ -6607,7 +6544,7 @@
       </c>
       <c r="M17" s="140"/>
       <c r="N17" s="169">
-        <v>1.8420000000000001E-3</v>
+        <v>1.8370000000000001E-3</v>
       </c>
       <c r="O17" s="170">
         <f>_xll.qlSimpleQuoteSetValue(D17,ROUND(N17,6),EvaluationDate)</f>
@@ -6639,7 +6576,7 @@
       </c>
       <c r="J18" s="218">
         <f>ROUND(Depo_Calculation!$I37,6)</f>
-        <v>1.8420000000000001E-3</v>
+        <v>1.8389999999999999E-3</v>
       </c>
       <c r="K18" s="156"/>
       <c r="L18" s="166">
@@ -6647,7 +6584,7 @@
       </c>
       <c r="M18" s="140"/>
       <c r="N18" s="169">
-        <v>1.8420000000000001E-3</v>
+        <v>1.8389999999999999E-3</v>
       </c>
       <c r="O18" s="170">
         <f>_xll.qlSimpleQuoteSetValue(D18,ROUND(N18,6),EvaluationDate)</f>
@@ -6679,7 +6616,7 @@
       </c>
       <c r="J19" s="218">
         <f>ROUND(Depo_Calculation!$I38,6)</f>
-        <v>1.8420000000000001E-3</v>
+        <v>1.843E-3</v>
       </c>
       <c r="K19" s="156"/>
       <c r="L19" s="166">
@@ -6687,7 +6624,7 @@
       </c>
       <c r="M19" s="140"/>
       <c r="N19" s="169">
-        <v>1.8420000000000001E-3</v>
+        <v>1.843E-3</v>
       </c>
       <c r="O19" s="170">
         <f>_xll.qlSimpleQuoteSetValue(D19,ROUND(N19,6),EvaluationDate)</f>
@@ -6719,7 +6656,7 @@
       </c>
       <c r="J20" s="218">
         <f>ROUND(Depo_Calculation!$I39,6)</f>
-        <v>1.8420000000000001E-3</v>
+        <v>1.843E-3</v>
       </c>
       <c r="K20" s="156"/>
       <c r="L20" s="166">
@@ -6727,7 +6664,7 @@
       </c>
       <c r="M20" s="140"/>
       <c r="N20" s="169">
-        <v>1.8420000000000001E-3</v>
+        <v>1.843E-3</v>
       </c>
       <c r="O20" s="170">
         <f>_xll.qlSimpleQuoteSetValue(D20,ROUND(N20,6),EvaluationDate)</f>
@@ -6759,7 +6696,7 @@
       </c>
       <c r="J21" s="218">
         <f>ROUND(Depo_Calculation!$I40,6)</f>
-        <v>1.8420000000000001E-3</v>
+        <v>1.818E-3</v>
       </c>
       <c r="K21" s="156"/>
       <c r="L21" s="166">
@@ -6767,7 +6704,7 @@
       </c>
       <c r="M21" s="140"/>
       <c r="N21" s="169">
-        <v>1.8420000000000001E-3</v>
+        <v>1.818E-3</v>
       </c>
       <c r="O21" s="170">
         <f>_xll.qlSimpleQuoteSetValue(D21,ROUND(N21,6),EvaluationDate)</f>
@@ -6799,7 +6736,7 @@
       </c>
       <c r="J22" s="218">
         <f>ROUND(Depo_Calculation!$I41,6)</f>
-        <v>1.8420000000000001E-3</v>
+        <v>1.818E-3</v>
       </c>
       <c r="K22" s="156"/>
       <c r="L22" s="166">
@@ -6807,7 +6744,7 @@
       </c>
       <c r="M22" s="140"/>
       <c r="N22" s="169">
-        <v>1.8420000000000001E-3</v>
+        <v>1.818E-3</v>
       </c>
       <c r="O22" s="170">
         <f>_xll.qlSimpleQuoteSetValue(D22,ROUND(N22,6),EvaluationDate)</f>
@@ -6839,7 +6776,7 @@
       </c>
       <c r="J23" s="218">
         <f>ROUND(Depo_Calculation!$I42,6)</f>
-        <v>1.8420000000000001E-3</v>
+        <v>1.818E-3</v>
       </c>
       <c r="K23" s="156"/>
       <c r="L23" s="166">
@@ -6847,7 +6784,7 @@
       </c>
       <c r="M23" s="140"/>
       <c r="N23" s="169">
-        <v>1.8420000000000001E-3</v>
+        <v>1.818E-3</v>
       </c>
       <c r="O23" s="170">
         <f>_xll.qlSimpleQuoteSetValue(D23,ROUND(N23,6),EvaluationDate)</f>
@@ -6879,7 +6816,7 @@
       </c>
       <c r="J24" s="219">
         <f>ROUND(Depo_Calculation!$I43,6)</f>
-        <v>1.817E-3</v>
+        <v>1.818E-3</v>
       </c>
       <c r="K24" s="211"/>
       <c r="L24" s="168">
@@ -6887,7 +6824,7 @@
       </c>
       <c r="M24" s="212"/>
       <c r="N24" s="172">
-        <v>1.817E-3</v>
+        <v>1.818E-3</v>
       </c>
       <c r="O24" s="170">
         <f>_xll.qlSimpleQuoteSetValue(D24,ROUND(N24,6),EvaluationDate)</f>
@@ -6922,7 +6859,7 @@
       </c>
       <c r="J25" s="217">
         <f>ROUND(Depo_Calculation!$J34,6)</f>
-        <v>3.382E-3</v>
+        <v>3.3790000000000001E-3</v>
       </c>
       <c r="K25" s="156"/>
       <c r="L25" s="237">
@@ -6930,7 +6867,7 @@
       </c>
       <c r="M25" s="140"/>
       <c r="N25" s="238">
-        <v>3.382E-3</v>
+        <v>3.3790000000000001E-3</v>
       </c>
       <c r="O25" s="239">
         <f>_xll.qlSimpleQuoteSetValue(D25,ROUND(N25,6),EvaluationDate)</f>
@@ -6938,7 +6875,7 @@
       </c>
       <c r="P25" s="190">
         <f>_xll.ohTrigger(O25:O40)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="231" customFormat="1" x14ac:dyDescent="0.2">
@@ -6969,7 +6906,7 @@
       </c>
       <c r="J26" s="218">
         <f>ROUND(Depo_Calculation!$J35,6)</f>
-        <v>3.382E-3</v>
+        <v>3.3790000000000001E-3</v>
       </c>
       <c r="K26" s="156"/>
       <c r="L26" s="166">
@@ -6977,7 +6914,7 @@
       </c>
       <c r="M26" s="140"/>
       <c r="N26" s="169">
-        <v>3.382E-3</v>
+        <v>3.3790000000000001E-3</v>
       </c>
       <c r="O26" s="170">
         <f>_xll.qlSimpleQuoteSetValue(D26,ROUND(N26,6),EvaluationDate)</f>
@@ -7010,7 +6947,7 @@
       </c>
       <c r="J27" s="218">
         <f>ROUND(Depo_Calculation!$J36,6)</f>
-        <v>3.382E-3</v>
+        <v>3.3800000000000002E-3</v>
       </c>
       <c r="K27" s="156"/>
       <c r="L27" s="166">
@@ -7018,7 +6955,7 @@
       </c>
       <c r="M27" s="140"/>
       <c r="N27" s="169">
-        <v>3.382E-3</v>
+        <v>3.3800000000000002E-3</v>
       </c>
       <c r="O27" s="170">
         <f>_xll.qlSimpleQuoteSetValue(D27,ROUND(N27,6),EvaluationDate)</f>
@@ -7050,7 +6987,7 @@
       </c>
       <c r="J28" s="218">
         <f>ROUND(Depo_Calculation!$J37,6)</f>
-        <v>3.382E-3</v>
+        <v>3.3809999999999999E-3</v>
       </c>
       <c r="K28" s="156"/>
       <c r="L28" s="166">
@@ -7058,7 +6995,7 @@
       </c>
       <c r="M28" s="140"/>
       <c r="N28" s="169">
-        <v>3.382E-3</v>
+        <v>3.3809999999999999E-3</v>
       </c>
       <c r="O28" s="170">
         <f>_xll.qlSimpleQuoteSetValue(D28,ROUND(N28,6),EvaluationDate)</f>
@@ -7090,7 +7027,7 @@
       </c>
       <c r="J29" s="218">
         <f>ROUND(Depo_Calculation!$J38,6)</f>
-        <v>3.382E-3</v>
+        <v>3.385E-3</v>
       </c>
       <c r="K29" s="156"/>
       <c r="L29" s="166">
@@ -7098,7 +7035,7 @@
       </c>
       <c r="M29" s="140"/>
       <c r="N29" s="169">
-        <v>3.382E-3</v>
+        <v>3.385E-3</v>
       </c>
       <c r="O29" s="170">
         <f>_xll.qlSimpleQuoteSetValue(D29,ROUND(N29,6),EvaluationDate)</f>
@@ -7130,7 +7067,7 @@
       </c>
       <c r="J30" s="218">
         <f>ROUND(Depo_Calculation!$J39,6)</f>
-        <v>3.382E-3</v>
+        <v>3.385E-3</v>
       </c>
       <c r="K30" s="156"/>
       <c r="L30" s="166">
@@ -7138,7 +7075,7 @@
       </c>
       <c r="M30" s="140"/>
       <c r="N30" s="169">
-        <v>3.382E-3</v>
+        <v>3.385E-3</v>
       </c>
       <c r="O30" s="170">
         <f>_xll.qlSimpleQuoteSetValue(D30,ROUND(N30,6),EvaluationDate)</f>
@@ -7170,7 +7107,7 @@
       </c>
       <c r="J31" s="218">
         <f>ROUND(Depo_Calculation!$J40,6)</f>
-        <v>3.382E-3</v>
+        <v>3.3600000000000001E-3</v>
       </c>
       <c r="K31" s="156"/>
       <c r="L31" s="166">
@@ -7178,7 +7115,7 @@
       </c>
       <c r="M31" s="140"/>
       <c r="N31" s="169">
-        <v>3.382E-3</v>
+        <v>3.3600000000000001E-3</v>
       </c>
       <c r="O31" s="170">
         <f>_xll.qlSimpleQuoteSetValue(D31,ROUND(N31,6),EvaluationDate)</f>
@@ -7210,7 +7147,7 @@
       </c>
       <c r="J32" s="218">
         <f>ROUND(Depo_Calculation!$J41,6)</f>
-        <v>3.382E-3</v>
+        <v>3.3600000000000001E-3</v>
       </c>
       <c r="K32" s="156"/>
       <c r="L32" s="166">
@@ -7218,7 +7155,7 @@
       </c>
       <c r="M32" s="140"/>
       <c r="N32" s="169">
-        <v>3.382E-3</v>
+        <v>3.3600000000000001E-3</v>
       </c>
       <c r="O32" s="170">
         <f>_xll.qlSimpleQuoteSetValue(D32,ROUND(N32,6),EvaluationDate)</f>
@@ -7250,7 +7187,7 @@
       </c>
       <c r="J33" s="218">
         <f>ROUND(Depo_Calculation!$J42,6)</f>
-        <v>3.382E-3</v>
+        <v>3.3600000000000001E-3</v>
       </c>
       <c r="K33" s="156"/>
       <c r="L33" s="166">
@@ -7258,7 +7195,7 @@
       </c>
       <c r="M33" s="140"/>
       <c r="N33" s="169">
-        <v>3.382E-3</v>
+        <v>3.3600000000000001E-3</v>
       </c>
       <c r="O33" s="170">
         <f>_xll.qlSimpleQuoteSetValue(D33,ROUND(N33,6),EvaluationDate)</f>
@@ -7290,7 +7227,7 @@
       </c>
       <c r="J34" s="218">
         <f>ROUND(Depo_Calculation!$J43,6)</f>
-        <v>3.3570000000000002E-3</v>
+        <v>3.3600000000000001E-3</v>
       </c>
       <c r="K34" s="156"/>
       <c r="L34" s="166">
@@ -7298,7 +7235,7 @@
       </c>
       <c r="M34" s="140"/>
       <c r="N34" s="169">
-        <v>3.3570000000000002E-3</v>
+        <v>3.3600000000000001E-3</v>
       </c>
       <c r="O34" s="170">
         <f>_xll.qlSimpleQuoteSetValue(D34,ROUND(N34,6),EvaluationDate)</f>
@@ -7330,7 +7267,7 @@
       </c>
       <c r="J35" s="218">
         <f>ROUND(Depo_Calculation!$J44,6)</f>
-        <v>3.349E-3</v>
+        <v>3.3630000000000001E-3</v>
       </c>
       <c r="K35" s="156"/>
       <c r="L35" s="166">
@@ -7338,7 +7275,7 @@
       </c>
       <c r="M35" s="140"/>
       <c r="N35" s="169">
-        <v>3.349E-3</v>
+        <v>3.3630000000000001E-3</v>
       </c>
       <c r="O35" s="170">
         <f>_xll.qlSimpleQuoteSetValue(D35,ROUND(N35,6),EvaluationDate)</f>
@@ -7370,7 +7307,7 @@
       </c>
       <c r="J36" s="218">
         <f>ROUND(Depo_Calculation!$J45,6)</f>
-        <v>3.3530000000000001E-3</v>
+        <v>3.3639999999999998E-3</v>
       </c>
       <c r="K36" s="156"/>
       <c r="L36" s="166">
@@ -7378,7 +7315,7 @@
       </c>
       <c r="M36" s="140"/>
       <c r="N36" s="169">
-        <v>3.3530000000000001E-3</v>
+        <v>3.3639999999999998E-3</v>
       </c>
       <c r="O36" s="170">
         <f>_xll.qlSimpleQuoteSetValue(D36,ROUND(N36,6),EvaluationDate)</f>
@@ -7410,7 +7347,7 @@
       </c>
       <c r="J37" s="218">
         <f>ROUND(Depo_Calculation!$J46,6)</f>
-        <v>3.3570000000000002E-3</v>
+        <v>3.3600000000000001E-3</v>
       </c>
       <c r="K37" s="156"/>
       <c r="L37" s="166">
@@ -7418,7 +7355,7 @@
       </c>
       <c r="M37" s="140"/>
       <c r="N37" s="169">
-        <v>3.3570000000000002E-3</v>
+        <v>3.3600000000000001E-3</v>
       </c>
       <c r="O37" s="170">
         <f>_xll.qlSimpleQuoteSetValue(D37,ROUND(N37,6),EvaluationDate)</f>
@@ -7450,7 +7387,7 @@
       </c>
       <c r="J38" s="218">
         <f>ROUND(Depo_Calculation!$J47,6)</f>
-        <v>3.3579999999999999E-3</v>
+        <v>3.3509999999999998E-3</v>
       </c>
       <c r="K38" s="156"/>
       <c r="L38" s="166">
@@ -7458,7 +7395,7 @@
       </c>
       <c r="M38" s="140"/>
       <c r="N38" s="169">
-        <v>3.3579999999999999E-3</v>
+        <v>3.3509999999999998E-3</v>
       </c>
       <c r="O38" s="170">
         <f>_xll.qlSimpleQuoteSetValue(D38,ROUND(N38,6),EvaluationDate)</f>
@@ -7490,7 +7427,7 @@
       </c>
       <c r="J39" s="218">
         <f>ROUND(Depo_Calculation!$J48,6)</f>
-        <v>3.3570000000000002E-3</v>
+        <v>3.3419999999999999E-3</v>
       </c>
       <c r="K39" s="156"/>
       <c r="L39" s="166">
@@ -7498,7 +7435,7 @@
       </c>
       <c r="M39" s="140"/>
       <c r="N39" s="169">
-        <v>3.3570000000000002E-3</v>
+        <v>3.3419999999999999E-3</v>
       </c>
       <c r="O39" s="170">
         <f>_xll.qlSimpleQuoteSetValue(D39,ROUND(N39,6),EvaluationDate)</f>
@@ -7530,7 +7467,7 @@
       </c>
       <c r="J40" s="219">
         <f>ROUND(Depo_Calculation!$J49,6)</f>
-        <v>3.3570000000000002E-3</v>
+        <v>3.336E-3</v>
       </c>
       <c r="K40" s="211"/>
       <c r="L40" s="168">
@@ -7538,7 +7475,7 @@
       </c>
       <c r="M40" s="212"/>
       <c r="N40" s="172">
-        <v>3.3570000000000002E-3</v>
+        <v>3.336E-3</v>
       </c>
       <c r="O40" s="170">
         <f>_xll.qlSimpleQuoteSetValue(D40,ROUND(N40,6),EvaluationDate)</f>

</xml_diff>